<commit_message>
fixed another bug with timestamps
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/SKO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8ED6E9A5-B3A5-524A-9159-697D4EFDA188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F188209-6169-3344-93C5-0BC281CCB4B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="480" windowWidth="26500" windowHeight="16220" activeTab="5" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
@@ -1127,10 +1127,10 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1300,7 +1300,7 @@
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
-IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date))+(uniform(1,",H3,", random(",P3,"))))"),
+IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("rpad(lpad(uniform(1,",H3," , random(",P3,"))::varchar, length(",H3,"),'0'),",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 ""))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
@@ -1370,10 +1370,10 @@
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1556,7 +1556,7 @@
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
-IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date))+(uniform(1,",H3,", random(",P3,"))))"),
+IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("rpad(lpad(uniform(1,",H3," , random(",P3,"))::varchar, length(",H3,"),'0'),",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 ""))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
@@ -1647,7 +1647,7 @@
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1824,7 +1824,7 @@
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
-IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date))+(uniform(1,",H3,", random(",P3,"))))"),
+IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("rpad(lpad(uniform(1,",H3," , random(",P3,"))::varchar, length(",H3,"),'0'),",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 ""))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
@@ -1941,7 +1941,7 @@
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
-IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date))+(uniform(1,",H4,", random(",P4,"))))"),
+IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("rpad(lpad(uniform(1,",H4," , random(",P4,"))::varchar, length(",H4,"),'0'),",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 ""))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),

</xml_diff>

<commit_message>
fixed problems in spreadsheet
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68A46ED2-5337-C34C-89EF-E4C930432789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12D7A7F8-9C70-7F4A-84B4-2E8E04E6AB7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="480" windowWidth="26500" windowHeight="16220" activeTab="2" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="840" yWindow="480" windowWidth="26500" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
     <sheet name="Customer Data" sheetId="16" r:id="rId2"/>
-    <sheet name="Cleansed Customer Data" sheetId="17" r:id="rId3"/>
+    <sheet name="datageneration_sample_spreadshe" sheetId="17" r:id="rId3"/>
     <sheet name="Formulas" sheetId="2" r:id="rId4"/>
     <sheet name="NULL Values Example" sheetId="9" r:id="rId5"/>
     <sheet name="Distributions" sheetId="14" r:id="rId6"/>
@@ -1187,7 +1187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2F4A9-4178-7746-B810-92567ADD6A96}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1509,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
support transient tables and fix double quotes problem in python
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12D7A7F8-9C70-7F4A-84B4-2E8E04E6AB7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01C091B-3AF8-634E-A24E-A916DFC4F2D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="480" windowWidth="26500" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
@@ -1513,7 +1513,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z2" sqref="Z2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1673,8 +1673,8 @@
         <v>|table1|</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists schema1;  create or replace table schema1.|table1| as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
+        <v>create schema if not exists schema1;  create or replace transient table schema1.|table1| as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -1766,7 +1766,7 @@
         <v>|table1|</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D11" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D11" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace transient table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
@@ -2443,10 +2443,10 @@
   <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2611,8 +2611,8 @@
         <v>table</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists schema;  create or replace table schema.table as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
+        <v>create schema if not exists schema;  create or replace transient table schema.table as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -2719,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AC2046-8798-C848-AA97-D3B5154A7925}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2879,8 +2879,8 @@
         <v>child</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists dbo;  create or replace table dbo.child as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
+        <v>create schema if not exists dbo;  create or replace transient table dbo.child as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -2996,7 +2996,7 @@
         <v>child</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D5" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D5" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace transient table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>create schema if not exists dbo;  create or replace table dbo.parent as select</v>
+        <v>create schema if not exists dbo;  create or replace transient table dbo.parent as select</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
adding transient,data_Retention_time_in_days to schema
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B72888A-FB9E-6E4B-8583-E0470032AEBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50261CF2-F009-5A47-A9C8-70893848955B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="26500" windowHeight="16220" activeTab="4" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="26500" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -1778,11 +1778,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1937,8 +1937,8 @@
         <v>table1</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists schema1;  create or replace transient table schema1.table1 as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create transient schema if not exists ",B3," data_retention_time_in_days=0;  create or replace table ",B3,".",C3," as select"))</f>
+        <v>create transient schema if not exists schema1 data_retention_time_in_days=0;  create or replace table schema1.table1 as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -2034,7 +2034,7 @@
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace transient table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
@@ -3672,11 +3672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD38527B-8DA9-F048-9888-D8112A4B2F49}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3841,8 +3841,8 @@
         <v>table1</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists schema1;  create or replace transient table schema1.table1 as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create transient schema if not exists ",B3," data_retention_time_in_days=0;  create or replace table ",B3,".",C3," as select"))</f>
+        <v>create transient schema if not exists schema1 data_retention_time_in_days=0;  create or replace table schema1.table1 as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -3947,7 +3947,7 @@
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace transient table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
@@ -5724,7 +5724,7 @@
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5883,8 +5883,8 @@
         <v>child</v>
       </c>
       <c r="D3" s="4" t="str">
-        <f>IF(C2=C3,"",_xlfn.CONCAT("create schema if not exists ",B3,";  create or replace transient table ",B3,".",C3," as select"))</f>
-        <v>create schema if not exists dbo;  create or replace transient table dbo.child as select</v>
+        <f>IF(C2=C3,"",_xlfn.CONCAT("create transient schema if not exists ",B3," data_retention_time_in_days=0;  create or replace table ",B3,".",C3," as select"))</f>
+        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.child as select</v>
       </c>
       <c r="E3" t="str">
         <f>IF(C3=C4,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K3,"))"))</f>
@@ -6001,7 +6001,7 @@
         <v>child</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D5" si="3">IF(C3=C4,"",_xlfn.CONCAT("create schema if not exists ",B4,";  create or replace transient table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D5" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>create schema if not exists dbo;  create or replace transient table dbo.parent as select</v>
+        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.parent as select</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
added normal distribution for char and varchar
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50261CF2-F009-5A47-A9C8-70893848955B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D85A381-48FF-0445-8BBF-B8A050112995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="26500" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="5" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="80">
   <si>
     <t>TableName</t>
   </si>
@@ -1778,11 +1778,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1951,14 +1951,16 @@
       <c r="G3" t="str">
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
-IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/10)))"),
+IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
+IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L3,
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -2048,14 +2050,16 @@
       <c r="G4" t="str">
         <f t="shared" ref="G4:G22" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
-IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/10)))"),
+IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
+IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L4,
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -3673,10 +3677,10 @@
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:D22"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3855,14 +3859,16 @@
       <c r="G3" t="str">
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
-IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/10)))"),
+IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
+IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L3,
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -3961,14 +3967,16 @@
       <c r="G4" t="str">
         <f t="shared" ref="G4:G22" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
-IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/10)))"),
+IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
+IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L4,
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -4810,11 +4818,11 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20011)) &gt; 300 then column101 else null end)::date as column101</v>
+        <v>column101::date as column101</v>
       </c>
       <c r="J13">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K13">
         <f t="shared" si="10"/>
@@ -4860,9 +4868,7 @@
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
@@ -4903,11 +4909,11 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20012)) &gt; 300 then column102 else null end)::timestamp as column102</v>
+        <v>column102::timestamp as column102</v>
       </c>
       <c r="J14">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" si="10"/>
@@ -4953,9 +4959,7 @@
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z14" s="12"/>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
@@ -4996,11 +5000,11 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20013)) &gt; 300 then column103 else null end)::varchar(10) as column103</v>
+        <v>column103::varchar(10) as column103</v>
       </c>
       <c r="J15">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="10"/>
@@ -5048,9 +5052,7 @@
         <v>10</v>
       </c>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
@@ -5091,11 +5093,11 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20014)) &gt; 300 then column104 else null end)::char(10) as column104</v>
+        <v>column104::char(10) as column104</v>
       </c>
       <c r="J16">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <f t="shared" si="10"/>
@@ -5143,9 +5145,7 @@
         <v>10</v>
       </c>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
@@ -5186,11 +5186,11 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20015)) &gt; 300 then column105 else null end)::bigint as column105</v>
+        <v>column105::bigint as column105</v>
       </c>
       <c r="J17">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <f t="shared" si="10"/>
@@ -5236,9 +5236,7 @@
       </c>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
@@ -5279,11 +5277,11 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20016)) &gt; 300 then column106 else null end)::integer as column106</v>
+        <v>column106::integer as column106</v>
       </c>
       <c r="J18">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <f t="shared" si="10"/>
@@ -5329,9 +5327,7 @@
       </c>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
-      <c r="Z18" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
       <c r="AC18" s="12"/>
@@ -5372,11 +5368,11 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20017)) &gt; 300 then column107 else null end)::double as column107</v>
+        <v>column107::double as column107</v>
       </c>
       <c r="J19">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <f t="shared" si="10"/>
@@ -5422,9 +5418,7 @@
       </c>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
-      <c r="Z19" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
@@ -5465,11 +5459,11 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20018)) &gt; 300 then column108 else null end)::float as column108</v>
+        <v>column108::float as column108</v>
       </c>
       <c r="J20">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <f t="shared" si="10"/>
@@ -5515,9 +5509,7 @@
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
-      <c r="Z20" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
       <c r="AC20" s="12"/>
@@ -5558,11 +5550,11 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20019)) &gt; 300 then column109 else null end)::number(10,2) as column109</v>
+        <v>column109::number(10,2) as column109</v>
       </c>
       <c r="J21">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <f t="shared" si="10"/>
@@ -5612,9 +5604,7 @@
       <c r="Y21" s="12">
         <v>2</v>
       </c>
-      <c r="Z21" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
@@ -5655,11 +5645,11 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20020)) &gt; 300 then column110 else null end)::integer as column110</v>
+        <v>column110::integer as column110</v>
       </c>
       <c r="J22">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <f t="shared" si="10"/>
@@ -5705,9 +5695,7 @@
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
-      <c r="Z22" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
@@ -5721,10 +5709,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AC2046-8798-C848-AA97-D3B5154A7925}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5734,7 +5722,7 @@
     <col min="4" max="4" width="85.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="84.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.5" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
@@ -5897,18 +5885,20 @@
       <c r="G3" t="str">
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
-IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/10)))"),
+IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
+IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L3,
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
-        <v>abs(trunc((5+normal(0,1,random(10001)))*(100/10)))::bigint as normal</v>
+        <v>abs(trunc((5+normal(0,1,random(10001)))*(100/20)))::bigint as normal</v>
       </c>
       <c r="H3">
         <f>U3</f>
@@ -5933,13 +5923,13 @@
         <f>IF(OR(OR(W3="timestamp(3)",W3="timestamp(6)"),W3="timestamp(9)"),"TIMESTAMP",W3)</f>
         <v>bigint</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="str">
         <f>IF(ISBLANK(X3),"",X3)</f>
-        <v>6</v>
-      </c>
-      <c r="N3">
+        <v/>
+      </c>
+      <c r="N3" t="str">
         <f>IF(ISBLANK(Y3),"",Y3)</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="O3">
         <f>O2+1</f>
@@ -5971,12 +5961,8 @@
       <c r="W3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="12">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="12">
-        <v>2</v>
-      </c>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
       <c r="AA3" s="12">
         <v>1</v>
@@ -5989,87 +5975,89 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <f t="shared" ref="A4:A5" si="0">A3+1</f>
+        <f t="shared" ref="A4:A7" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B5" si="1">R4</f>
+        <f t="shared" ref="B4:B7" si="1">R4</f>
         <v>dbo</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C5" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C7" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>child</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D5" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D7" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E5" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <f t="shared" ref="E4:E7" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F5" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
-        <v>uniform</v>
+        <f t="shared" ref="F4:F7" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <v>normal</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G5" si="6">_xlfn.CONCAT(
+        <f t="shared" ref="G4:G7" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
-IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/10)))"),
+IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
+IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))),"::",L4,
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
-        <v>uniform(1,100 , random(10002))::bigint as uniform</v>
+        <v>rpad(abs(trunc((5+normal(0,1,random(10002)))*(100/20)))::varchar,6,'abcdefghifklmnopqrstuvwxyz')::char(6) as normal</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H5" si="7">U4</f>
+        <f t="shared" ref="H4:H7" si="7">U4</f>
         <v>100</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I5" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
+        <f t="shared" ref="I4:I7" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
-        <v>uniform::bigint as uniform</v>
+        <v>normal::char(6) as normal</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J5" si="9">IF((Z4=0),0,INT((Z4/V4)*1000))</f>
+        <f t="shared" ref="J4:J7" si="9">IF((Z4=0),0,INT((Z4/V4)*1000))</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K5" si="10">V4</f>
+        <f t="shared" ref="K4:K7" si="10">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L5" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
-        <v>bigint</v>
+        <f t="shared" ref="L4:L7" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
+        <v>char</v>
       </c>
       <c r="M4">
-        <f>IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M7" si="12">IF(ISBLANK(X4),"",X4)</f>
         <v>6</v>
       </c>
-      <c r="N4">
-        <f>IF(ISBLANK(Y4),"",Y4)</f>
-        <v>2</v>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N7" si="13">IF(ISBLANK(Y4),"",Y4)</f>
+        <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O5" si="12">O3+1</f>
+        <f t="shared" ref="O4:O7" si="14">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P5" si="13">P3+1</f>
+        <f t="shared" ref="P4:P7" si="15">P3+1</f>
         <v>10002</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q5" si="14">AA4</f>
-        <v>0</v>
+        <f t="shared" ref="Q4:Q7" si="16">AA4</f>
+        <v>1</v>
       </c>
       <c r="R4" s="12" t="s">
         <v>12</v>
@@ -6078,7 +6066,7 @@
         <v>36</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U4" s="12">
         <v>100</v>
@@ -6087,16 +6075,16 @@
         <v>10000</v>
       </c>
       <c r="W4" s="12" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="X4" s="12">
         <v>6</v>
       </c>
-      <c r="Y4" s="12">
-        <v>2</v>
-      </c>
+      <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
-      <c r="AA4" s="12"/>
+      <c r="AA4" s="12">
+        <v>1</v>
+      </c>
       <c r="AB4" s="12" t="s">
         <v>10</v>
       </c>
@@ -6114,23 +6102,23 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="2"/>
-        <v>parent</v>
+        <v>child</v>
       </c>
       <c r="D5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.parent as select</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 100))</v>
+        <v/>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="5"/>
-        <v>id</v>
+        <v>normal</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>seq8()::bigint as id</v>
+        <v>rpad(abs(trunc((5+normal(0,1,random(10003)))*(100/20)))::varchar,uniform(length(100),6,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(6) as normal</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
@@ -6138,7 +6126,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="8"/>
-        <v>id::bigint as id</v>
+        <v>normal::varchar(6) as normal</v>
       </c>
       <c r="J5">
         <f t="shared" si="9"/>
@@ -6146,55 +6134,259 @@
       </c>
       <c r="K5">
         <f t="shared" si="10"/>
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" ref="M5" si="15">IF(ISBLANK(X5),"",X5)</f>
+        <v>varchar</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="O5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>20003</v>
       </c>
       <c r="P5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>10003</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>1</v>
       </c>
       <c r="R5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="U5" s="12">
         <v>100</v>
       </c>
       <c r="V5" s="12">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X5" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="X5" s="12">
+        <v>6</v>
+      </c>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
+      <c r="AA5" s="12">
+        <v>1</v>
+      </c>
       <c r="AB5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="1"/>
+        <v>dbo</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="2"/>
+        <v>child</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="5"/>
+        <v>uniform</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="6"/>
+        <v>uniform(1,100 , random(10004))::bigint as uniform</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="8"/>
+        <v>uniform::bigint as uniform</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="11"/>
+        <v>bigint</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O6">
+        <f t="shared" si="14"/>
+        <v>20004</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="15"/>
+        <v>10004</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U6" s="12">
+        <v>100</v>
+      </c>
+      <c r="V6" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X6" s="12">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="1"/>
+        <v>dbo</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="2"/>
+        <v>parent</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.parent as select</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 100))</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="5"/>
+        <v>id</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="6"/>
+        <v>seq8()::bigint as id</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="8"/>
+        <v>id::bigint as id</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="11"/>
+        <v>bigint</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O7">
+        <f t="shared" si="14"/>
+        <v>20005</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="15"/>
+        <v>10005</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" s="12">
+        <v>100</v>
+      </c>
+      <c r="V7" s="12">
+        <v>100</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated documentation; added unique columns for bigint & char; better error handling
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D85A381-48FF-0445-8BBF-B8A050112995}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE6CC5A0-2342-8644-B746-5E58200F79AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="5" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="4" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="85">
   <si>
     <t>TableName</t>
   </si>
@@ -302,6 +302,21 @@
   </si>
   <si>
     <t>column110</t>
+  </si>
+  <si>
+    <t>column11</t>
+  </si>
+  <si>
+    <t>column12</t>
+  </si>
+  <si>
+    <t>column111</t>
+  </si>
+  <si>
+    <t>column112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
   </si>
 </sst>
 </file>
@@ -360,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -409,11 +424,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -443,6 +469,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -789,51 +816,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
@@ -877,149 +904,149 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="34" customHeight="1">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="34" customHeight="1">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" ht="34" customHeight="1">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="34" customHeight="1">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" ht="34" customHeight="1">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="34" customHeight="1">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" ht="34" customHeight="1">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:13" ht="34" customHeight="1">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1109,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2F4A9-4178-7746-B810-92567ADD6A96}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M22"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1184,7 +1211,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E3" s="12">
         <v>10000</v>
@@ -1213,7 +1240,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E4" s="12">
         <v>10000</v>
@@ -1242,7 +1269,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E5" s="12">
         <v>10000</v>
@@ -1273,7 +1300,7 @@
         <v>52</v>
       </c>
       <c r="D6" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E6" s="12">
         <v>10000</v>
@@ -1304,7 +1331,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E7" s="12">
         <v>10000</v>
@@ -1333,7 +1360,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E8" s="12">
         <v>10000</v>
@@ -1362,7 +1389,7 @@
         <v>60</v>
       </c>
       <c r="D9" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E9" s="12">
         <v>10000</v>
@@ -1391,7 +1418,7 @@
         <v>61</v>
       </c>
       <c r="D10" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E10" s="12">
         <v>10000</v>
@@ -1420,7 +1447,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E11" s="12">
         <v>10000</v>
@@ -1453,19 +1480,19 @@
         <v>78</v>
       </c>
       <c r="D12" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E12" s="12">
         <v>10000</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="G12" s="12">
+        <v>10</v>
+      </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
@@ -1479,22 +1506,20 @@
         <v>48</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D13" s="12">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E13" s="12">
         <v>10000</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12">
-        <v>3000</v>
-      </c>
+      <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -1508,21 +1533,21 @@
         <v>48</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D14" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E14" s="12">
         <v>10000</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12">
-        <v>3000</v>
+      <c r="I14" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -1537,20 +1562,18 @@
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E15" s="12">
         <v>10000</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="12">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12">
         <v>3000</v>
@@ -1568,20 +1591,18 @@
         <v>48</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E16" s="12">
         <v>10000</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12">
         <v>3000</v>
@@ -1599,18 +1620,20 @@
         <v>48</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E17" s="12">
         <v>10000</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="G17" s="12">
+        <v>10</v>
+      </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12">
         <v>3000</v>
@@ -1628,18 +1651,20 @@
         <v>48</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D18" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E18" s="12">
         <v>10000</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="G18" s="12">
+        <v>10</v>
+      </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12">
         <v>3000</v>
@@ -1657,16 +1682,16 @@
         <v>48</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E19" s="12">
         <v>10000</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -1686,16 +1711,16 @@
         <v>48</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E20" s="12">
         <v>10000</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -1715,23 +1740,19 @@
         <v>48</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="E21" s="12">
         <v>10000</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="12">
-        <v>10</v>
-      </c>
-      <c r="H21" s="12">
-        <v>2</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="12">
         <v>3000</v>
       </c>
@@ -1748,16 +1769,16 @@
         <v>48</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D22" s="12">
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="E22" s="12">
         <v>10000</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -1768,6 +1789,128 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="12">
+        <v>1234</v>
+      </c>
+      <c r="E23" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="12">
+        <v>10</v>
+      </c>
+      <c r="H23" s="12">
+        <v>2</v>
+      </c>
+      <c r="I23" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="12">
+        <v>10</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1776,13 +1919,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G22"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1955,20 +2098,21 @@
 IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L3,
+""))))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
-        <v>dateadd(day,uniform(1,100 , random(10001)),current_date)::date as column1</v>
+        <v>dateadd(day,uniform(1,1234 , random(10001)),current_date)::date as column1</v>
       </c>
       <c r="H3">
         <f>U3</f>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K3">
         <f>V3</f>
@@ -2004,7 +2148,7 @@
         <v>49</v>
       </c>
       <c r="U3" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V3" s="12">
         <v>10000</v>
@@ -2024,73 +2168,74 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <f t="shared" ref="A4:A22" si="0">A3+1</f>
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B22" si="1">R4</f>
+        <f t="shared" ref="B4:B26" si="1">R4</f>
         <v>schema1</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C22" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C26" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D26" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E22" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <f t="shared" ref="E4:E26" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
         <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F22" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <f t="shared" ref="F4:F26" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
         <v>column2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G22" si="6">_xlfn.CONCAT(
+        <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
 IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L4,
+""))))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,100, random(10002))))::timestamp as column2</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10002))))::timestamp as column2</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H22" si="7">U4</f>
-        <v>100</v>
+        <f t="shared" ref="H4:H26" si="7">U4</f>
+        <v>1234</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K22" si="8">V4</f>
+        <f t="shared" ref="K4:K26" si="8">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L22" si="9">W4</f>
+        <f t="shared" ref="L4:L26" si="9">W4</f>
         <v>timestamp</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M22" si="10">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M26" si="10">IF(ISBLANK(X4),"",X4)</f>
         <v/>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N22" si="11">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N26" si="11">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O22" si="12">O3+1</f>
+        <f t="shared" ref="O4:O26" si="12">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P22" si="13">P3+1</f>
+        <f t="shared" ref="P4:P26" si="13">P3+1</f>
         <v>10002</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -2103,7 +2248,7 @@
         <v>50</v>
       </c>
       <c r="U4" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V4" s="12">
         <v>10000</v>
@@ -2148,11 +2293,11 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10003))::varchar,uniform(length(100),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>rpad(uniform(1,1234 , random(10003))::varchar,uniform(length(1234),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K5">
         <f t="shared" si="8"/>
@@ -2188,7 +2333,7 @@
         <v>51</v>
       </c>
       <c r="U5" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V5" s="12">
         <v>10000</v>
@@ -2235,11 +2380,11 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10004))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column4</v>
+        <v>rpad(uniform(1,1234 , random(10004))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column4</v>
       </c>
       <c r="H6">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K6">
         <f t="shared" si="8"/>
@@ -2275,7 +2420,7 @@
         <v>52</v>
       </c>
       <c r="U6" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V6" s="12">
         <v>10000</v>
@@ -2322,11 +2467,11 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10005))::bigint as column5</v>
+        <v>uniform(1,1234 , random(10005))::bigint as column5</v>
       </c>
       <c r="H7">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K7">
         <f t="shared" si="8"/>
@@ -2362,7 +2507,7 @@
         <v>53</v>
       </c>
       <c r="U7" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V7" s="12">
         <v>10000</v>
@@ -2407,11 +2552,11 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10006))::integer as column6</v>
+        <v>uniform(1,1234 , random(10006))::integer as column6</v>
       </c>
       <c r="H8">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K8">
         <f t="shared" si="8"/>
@@ -2447,7 +2592,7 @@
         <v>54</v>
       </c>
       <c r="U8" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V8" s="12">
         <v>10000</v>
@@ -2492,11 +2637,11 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10007))::double as column7</v>
+        <v>uniform(1,1234 , random(10007))::double as column7</v>
       </c>
       <c r="H9">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K9">
         <f t="shared" si="8"/>
@@ -2532,7 +2677,7 @@
         <v>60</v>
       </c>
       <c r="U9" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V9" s="12">
         <v>10000</v>
@@ -2577,11 +2722,11 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10008))::float as column8</v>
+        <v>uniform(1,1234 , random(10008))::float as column8</v>
       </c>
       <c r="H10">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K10">
         <f t="shared" si="8"/>
@@ -2617,7 +2762,7 @@
         <v>61</v>
       </c>
       <c r="U10" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V10" s="12">
         <v>10000</v>
@@ -2662,11 +2807,11 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10009))::number(10,2) as column9</v>
+        <v>uniform(1,1234 , random(10009))::number(10,2) as column9</v>
       </c>
       <c r="H11">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K11">
         <f t="shared" si="8"/>
@@ -2702,7 +2847,7 @@
         <v>64</v>
       </c>
       <c r="U11" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V11" s="12">
         <v>10000</v>
@@ -2751,11 +2896,11 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column10</v>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column10</v>
       </c>
       <c r="H12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="K12">
         <f t="shared" si="8"/>
@@ -2763,11 +2908,11 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="9"/>
-        <v>integer</v>
-      </c>
-      <c r="M12" t="str">
+        <v>char</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="10"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="11"/>
@@ -2791,19 +2936,19 @@
         <v>78</v>
       </c>
       <c r="U12" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V12" s="12">
         <v>10000</v>
       </c>
       <c r="W12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X12" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X12" s="12">
+        <v>10</v>
+      </c>
       <c r="Y12" s="12"/>
-      <c r="Z12" s="12" t="s">
-        <v>67</v>
-      </c>
+      <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
@@ -2832,15 +2977,15 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="5"/>
-        <v>column101</v>
+        <v>column11</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="6"/>
-        <v>dateadd(day,uniform(1,100 , random(10011)),current_date)::date as column101</v>
+        <v>seq8()::bigint as column11</v>
       </c>
       <c r="H13">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="K13">
         <f t="shared" si="8"/>
@@ -2848,7 +2993,7 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="9"/>
-        <v>date</v>
+        <v>bigint</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="10"/>
@@ -2873,22 +3018,20 @@
         <v>48</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="U13" s="12">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="V13" s="12">
         <v>10000</v>
       </c>
       <c r="W13" s="12" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
-      <c r="Z13" s="12">
-        <v>3000</v>
-      </c>
+      <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
@@ -2917,15 +3060,15 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="5"/>
-        <v>column102</v>
+        <v>column12</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="6"/>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,100, random(10012))))::timestamp as column102</v>
+        <v>null::integer as column12</v>
       </c>
       <c r="H14">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" si="8"/>
@@ -2933,7 +3076,7 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="9"/>
-        <v>timestamp</v>
+        <v>integer</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="10"/>
@@ -2958,21 +3101,21 @@
         <v>48</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="U14" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="V14" s="12">
         <v>10000</v>
       </c>
       <c r="W14" s="12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="12">
-        <v>3000</v>
+      <c r="Z14" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
@@ -3002,15 +3145,15 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="5"/>
-        <v>column103</v>
+        <v>column101</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10013))::varchar,uniform(length(100),10,random(10013+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>dateadd(day,uniform(1,1234 , random(10013)),current_date)::date as column101</v>
       </c>
       <c r="H15">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K15">
         <f t="shared" si="8"/>
@@ -3018,11 +3161,11 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="9"/>
-        <v>varchar</v>
-      </c>
-      <c r="M15">
+        <v>date</v>
+      </c>
+      <c r="M15" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="11"/>
@@ -3043,20 +3186,18 @@
         <v>48</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U15" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V15" s="12">
         <v>10000</v>
       </c>
       <c r="W15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X15" s="12">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
       <c r="Z15" s="12">
         <v>3000</v>
@@ -3089,15 +3230,15 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="5"/>
-        <v>column104</v>
+        <v>column102</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10014))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10014))))::timestamp as column102</v>
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K16">
         <f t="shared" si="8"/>
@@ -3105,11 +3246,11 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="9"/>
-        <v>char</v>
-      </c>
-      <c r="M16">
+        <v>timestamp</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="11"/>
@@ -3130,20 +3271,18 @@
         <v>48</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U16" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V16" s="12">
         <v>10000</v>
       </c>
       <c r="W16" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="X16" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
       <c r="Z16" s="12">
         <v>3000</v>
@@ -3176,15 +3315,15 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="5"/>
-        <v>column105</v>
+        <v>column103</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10015))::bigint as column105</v>
+        <v>rpad(uniform(1,1234 , random(10015))::varchar,uniform(length(1234),10,random(10015+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K17">
         <f t="shared" si="8"/>
@@ -3192,11 +3331,11 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="9"/>
-        <v>bigint</v>
-      </c>
-      <c r="M17" t="str">
+        <v>varchar</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="10"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="11"/>
@@ -3217,18 +3356,20 @@
         <v>48</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U17" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V17" s="12">
         <v>10000</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X17" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="X17" s="12">
+        <v>10</v>
+      </c>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12">
         <v>3000</v>
@@ -3261,15 +3402,15 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="5"/>
-        <v>column106</v>
+        <v>column104</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10016))::integer as column106</v>
+        <v>rpad(uniform(1,1234 , random(10016))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K18">
         <f t="shared" si="8"/>
@@ -3277,11 +3418,11 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="9"/>
-        <v>integer</v>
-      </c>
-      <c r="M18" t="str">
+        <v>char</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="10"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="11"/>
@@ -3302,18 +3443,20 @@
         <v>48</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U18" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V18" s="12">
         <v>10000</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X18" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X18" s="12">
+        <v>10</v>
+      </c>
       <c r="Y18" s="12"/>
       <c r="Z18" s="12">
         <v>3000</v>
@@ -3346,15 +3489,15 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="5"/>
-        <v>column107</v>
+        <v>column105</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10017))::double as column107</v>
+        <v>uniform(1,1234 , random(10017))::bigint as column105</v>
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K19">
         <f t="shared" si="8"/>
@@ -3362,7 +3505,7 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="9"/>
-        <v>double</v>
+        <v>bigint</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="10"/>
@@ -3387,16 +3530,16 @@
         <v>48</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U19" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V19" s="12">
         <v>10000</v>
       </c>
       <c r="W19" s="12" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
@@ -3431,15 +3574,15 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="5"/>
-        <v>column108</v>
+        <v>column106</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10018))::float as column108</v>
+        <v>uniform(1,1234 , random(10018))::integer as column106</v>
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K20">
         <f t="shared" si="8"/>
@@ -3447,7 +3590,7 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="9"/>
-        <v>float</v>
+        <v>integer</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="10"/>
@@ -3472,16 +3615,16 @@
         <v>48</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U20" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V20" s="12">
         <v>10000</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
@@ -3516,15 +3659,15 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="5"/>
-        <v>column109</v>
+        <v>column107</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10019))::number(10,2) as column109</v>
+        <v>uniform(1,1234 , random(10019))::double as column107</v>
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="K21">
         <f t="shared" si="8"/>
@@ -3532,15 +3675,15 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="9"/>
-        <v>number</v>
-      </c>
-      <c r="M21">
+        <v>double</v>
+      </c>
+      <c r="M21" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="N21">
+        <v/>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="O21">
         <f t="shared" si="12"/>
@@ -3557,23 +3700,19 @@
         <v>48</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U21" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V21" s="12">
         <v>10000</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X21" s="12">
-        <v>10</v>
-      </c>
-      <c r="Y21" s="12">
-        <v>2</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
       <c r="Z21" s="12">
         <v>3000</v>
       </c>
@@ -3601,19 +3740,19 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <v/>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="5"/>
-        <v>column110</v>
+        <v>column108</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column110</v>
+        <v>uniform(1,1234 , random(10020))::float as column108</v>
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="K22">
         <f t="shared" si="8"/>
@@ -3621,7 +3760,7 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="9"/>
-        <v>integer</v>
+        <v>float</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="10"/>
@@ -3646,16 +3785,16 @@
         <v>48</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U22" s="12">
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="V22" s="12">
         <v>10000</v>
       </c>
       <c r="W22" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
@@ -3666,6 +3805,352 @@
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="5"/>
+        <v>column109</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="6"/>
+        <v>uniform(1,1234 , random(10021))::number(10,2) as column109</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>1234</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="9"/>
+        <v>number</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="12"/>
+        <v>20021</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="13"/>
+        <v>10021</v>
+      </c>
+      <c r="R23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="12">
+        <v>1234</v>
+      </c>
+      <c r="V23" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X23" s="12">
+        <v>10</v>
+      </c>
+      <c r="Y23" s="12">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="5"/>
+        <v>column110</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="6"/>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="9"/>
+        <v>char</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O24">
+        <f t="shared" si="12"/>
+        <v>20022</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="13"/>
+        <v>10022</v>
+      </c>
+      <c r="R24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="V24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X24" s="12">
+        <v>10</v>
+      </c>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12"/>
+      <c r="AD24" s="12"/>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="5"/>
+        <v>column111</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="6"/>
+        <v>seq8()::bigint as column111</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="9"/>
+        <v>bigint</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O25">
+        <f t="shared" si="12"/>
+        <v>20023</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="13"/>
+        <v>10023</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="U25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="V25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AD25" s="12"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="5"/>
+        <v>column112</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="6"/>
+        <v>null::integer as column112</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="9"/>
+        <v>integer</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O26">
+        <f t="shared" si="12"/>
+        <v>20024</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="13"/>
+        <v>10024</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U26" s="12">
+        <v>0</v>
+      </c>
+      <c r="V26" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3674,13 +4159,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD38527B-8DA9-F048-9888-D8112A4B2F49}">
-  <dimension ref="A1:AD22"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G22"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3863,20 +4348,21 @@
 IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L3,
+""))))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
-        <v>dateadd(day,uniform(1,100 , random(10001)),current_date)::date as column1</v>
+        <v>dateadd(day,uniform(1,1234 , random(10001)),current_date)::date as column1</v>
       </c>
       <c r="H3">
         <f>U3</f>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I3" t="str">
         <f>_xlfn.CONCAT(IF(J3=0,F3,_xlfn.CONCAT("(case when uniform(1,1000,random(",O3,")) &gt; ",J3," then ",F3," else null end)")),"::",L3,
@@ -3886,7 +4372,7 @@
         <v>column1::date as column1</v>
       </c>
       <c r="J3">
-        <f>IF(ISBLANK(Z3),0,INT((Z3/V3)*1000))</f>
+        <f>IF(ISBLANK(Z3),0,IF(TRIM(Z3)="",0,INT((Z3/V3)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K3">
@@ -3923,7 +4409,7 @@
         <v>49</v>
       </c>
       <c r="U3" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V3" s="12">
         <v>10000</v>
@@ -3933,7 +4419,9 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
+      <c r="Z3" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA3" s="12"/>
       <c r="AB3" s="12"/>
       <c r="AC3" s="12"/>
@@ -3941,84 +4429,85 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <f t="shared" ref="A4:A22" si="0">A3+1</f>
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B22" si="1">R4</f>
+        <f t="shared" ref="B4:B26" si="1">R4</f>
         <v>schema1</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C22" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C26" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D22" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D26" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E22" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <f t="shared" ref="E4:E26" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
         <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F22" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <f t="shared" ref="F4:F26" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
         <v>column2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G22" si="6">_xlfn.CONCAT(
+        <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
 IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L4,
+""))))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,100, random(10002))))::timestamp as column2</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10002))))::timestamp as column2</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H22" si="7">U4</f>
-        <v>100</v>
+        <f t="shared" ref="H4:H26" si="7">U4</f>
+        <v>1234</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I22" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
+        <f t="shared" ref="I4:I26" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>column2::timestamp as column2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J22" si="9">IF(ISBLANK(Z4),0,INT((Z4/V4)*1000))</f>
+        <f t="shared" ref="J4:J26" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K22" si="10">V4</f>
+        <f t="shared" ref="K4:K26" si="10">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L22" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
+        <f t="shared" ref="L4:L26" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
         <v>timestamp</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M22" si="12">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M26" si="12">IF(ISBLANK(X4),"",X4)</f>
         <v/>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N22" si="13">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N26" si="13">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O22" si="14">O3+1</f>
+        <f t="shared" ref="O4:O26" si="14">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P22" si="15">P3+1</f>
+        <f t="shared" ref="P4:P26" si="15">P3+1</f>
         <v>10002</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -4031,7 +4520,7 @@
         <v>50</v>
       </c>
       <c r="U4" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V4" s="12">
         <v>10000</v>
@@ -4041,7 +4530,9 @@
       </c>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="Z4" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
@@ -4074,11 +4565,11 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10003))::varchar,uniform(length(100),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>rpad(uniform(1,1234 , random(10003))::varchar,uniform(length(1234),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="8"/>
@@ -4122,7 +4613,7 @@
         <v>51</v>
       </c>
       <c r="U5" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V5" s="12">
         <v>10000</v>
@@ -4134,7 +4625,9 @@
         <v>10</v>
       </c>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
+      <c r="Z5" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
@@ -4167,11 +4660,11 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10004))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column4</v>
+        <v>rpad(uniform(1,1234 , random(10004))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column4</v>
       </c>
       <c r="H6">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="8"/>
@@ -4215,7 +4708,7 @@
         <v>52</v>
       </c>
       <c r="U6" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V6" s="12">
         <v>10000</v>
@@ -4227,7 +4720,9 @@
         <v>10</v>
       </c>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
+      <c r="Z6" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
@@ -4260,11 +4755,11 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10005))::bigint as column5</v>
+        <v>uniform(1,1234 , random(10005))::bigint as column5</v>
       </c>
       <c r="H7">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="8"/>
@@ -4308,7 +4803,7 @@
         <v>53</v>
       </c>
       <c r="U7" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V7" s="12">
         <v>10000</v>
@@ -4318,7 +4813,9 @@
       </c>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="Z7" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
@@ -4351,11 +4848,11 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10006))::integer as column6</v>
+        <v>uniform(1,1234 , random(10006))::integer as column6</v>
       </c>
       <c r="H8">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="8"/>
@@ -4399,7 +4896,7 @@
         <v>54</v>
       </c>
       <c r="U8" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V8" s="12">
         <v>10000</v>
@@ -4409,7 +4906,9 @@
       </c>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
+      <c r="Z8" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
@@ -4442,11 +4941,11 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10007))::double as column7</v>
+        <v>uniform(1,1234 , random(10007))::double as column7</v>
       </c>
       <c r="H9">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="8"/>
@@ -4490,7 +4989,7 @@
         <v>60</v>
       </c>
       <c r="U9" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V9" s="12">
         <v>10000</v>
@@ -4500,7 +4999,9 @@
       </c>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
+      <c r="Z9" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
       <c r="AC9" s="12"/>
@@ -4533,11 +5034,11 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10008))::float as column8</v>
+        <v>uniform(1,1234 , random(10008))::float as column8</v>
       </c>
       <c r="H10">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="8"/>
@@ -4581,7 +5082,7 @@
         <v>61</v>
       </c>
       <c r="U10" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V10" s="12">
         <v>10000</v>
@@ -4591,7 +5092,9 @@
       </c>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
+      <c r="Z10" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
@@ -4624,11 +5127,11 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10009))::number(10,2) as column9</v>
+        <v>uniform(1,1234 , random(10009))::number(10,2) as column9</v>
       </c>
       <c r="H11">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="8"/>
@@ -4672,7 +5175,7 @@
         <v>64</v>
       </c>
       <c r="U11" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V11" s="12">
         <v>10000</v>
@@ -4686,7 +5189,9 @@
       <c r="Y11" s="12">
         <v>2</v>
       </c>
-      <c r="Z11" s="12"/>
+      <c r="Z11" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
@@ -4719,15 +5224,15 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column10</v>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column10</v>
       </c>
       <c r="H12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="8"/>
-        <v>column10::integer as column10</v>
+        <v>column10::char(10) as column10</v>
       </c>
       <c r="J12">
         <f t="shared" si="9"/>
@@ -4739,11 +5244,11 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="11"/>
-        <v>integer</v>
-      </c>
-      <c r="M12" t="str">
+        <v>char</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="13"/>
@@ -4767,15 +5272,17 @@
         <v>78</v>
       </c>
       <c r="U12" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V12" s="12">
         <v>10000</v>
       </c>
       <c r="W12" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X12" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X12" s="12">
+        <v>10</v>
+      </c>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
@@ -4806,19 +5313,19 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="5"/>
-        <v>column101</v>
+        <v>column11</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="6"/>
-        <v>dateadd(day,uniform(1,100 , random(10011)),current_date)::date as column101</v>
+        <v>seq8()::bigint as column11</v>
       </c>
       <c r="H13">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="8"/>
-        <v>column101::date as column101</v>
+        <v>column11::bigint as column11</v>
       </c>
       <c r="J13">
         <f t="shared" si="9"/>
@@ -4830,7 +5337,7 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="11"/>
-        <v>date</v>
+        <v>bigint</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="12"/>
@@ -4855,16 +5362,16 @@
         <v>48</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="U13" s="12">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="V13" s="12">
         <v>10000</v>
       </c>
       <c r="W13" s="12" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -4897,19 +5404,19 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="5"/>
-        <v>column102</v>
+        <v>column12</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="6"/>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,100, random(10012))))::timestamp as column102</v>
+        <v>null::integer as column12</v>
       </c>
       <c r="H14">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="8"/>
-        <v>column102::timestamp as column102</v>
+        <v>column12::integer as column12</v>
       </c>
       <c r="J14">
         <f t="shared" si="9"/>
@@ -4921,7 +5428,7 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="11"/>
-        <v>timestamp</v>
+        <v>integer</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="12"/>
@@ -4946,20 +5453,22 @@
         <v>48</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="U14" s="12">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="V14" s="12">
         <v>10000</v>
       </c>
       <c r="W14" s="12" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
+      <c r="Z14" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
@@ -4988,23 +5497,23 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="5"/>
-        <v>column103</v>
+        <v>column101</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10013))::varchar,uniform(length(100),10,random(10013+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>dateadd(day,uniform(1,1234 , random(10013)),current_date)::date as column101</v>
       </c>
       <c r="H15">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="8"/>
-        <v>column103::varchar(10) as column103</v>
+        <v>(case when uniform(1,1000,random(20013)) &gt; 300 then column101 else null end)::date as column101</v>
       </c>
       <c r="J15">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K15">
         <f t="shared" si="10"/>
@@ -5012,11 +5521,11 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="11"/>
-        <v>varchar</v>
-      </c>
-      <c r="M15">
+        <v>date</v>
+      </c>
+      <c r="M15" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="13"/>
@@ -5037,22 +5546,22 @@
         <v>48</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U15" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V15" s="12">
         <v>10000</v>
       </c>
       <c r="W15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X15" s="12">
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
+      <c r="Z15" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
@@ -5081,23 +5590,23 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="5"/>
-        <v>column104</v>
+        <v>column102</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,100 , random(10014))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10014))))::timestamp as column102</v>
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="8"/>
-        <v>column104::char(10) as column104</v>
+        <v>(case when uniform(1,1000,random(20014)) &gt; 300 then column102 else null end)::timestamp as column102</v>
       </c>
       <c r="J16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K16">
         <f t="shared" si="10"/>
@@ -5105,11 +5614,11 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="11"/>
-        <v>char</v>
-      </c>
-      <c r="M16">
+        <v>timestamp</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="13"/>
@@ -5130,22 +5639,22 @@
         <v>48</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U16" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V16" s="12">
         <v>10000</v>
       </c>
       <c r="W16" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="X16" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
+      <c r="Z16" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
@@ -5174,23 +5683,23 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="5"/>
-        <v>column105</v>
+        <v>column103</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10015))::bigint as column105</v>
+        <v>rpad(uniform(1,1234 , random(10015))::varchar,uniform(length(1234),10,random(10015+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="8"/>
-        <v>column105::bigint as column105</v>
+        <v>(case when uniform(1,1000,random(20015)) &gt; 300 then column103 else null end)::varchar(10) as column103</v>
       </c>
       <c r="J17">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K17">
         <f t="shared" si="10"/>
@@ -5198,11 +5707,11 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M17" t="str">
+        <v>varchar</v>
+      </c>
+      <c r="M17">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="13"/>
@@ -5223,20 +5732,24 @@
         <v>48</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U17" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V17" s="12">
         <v>10000</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X17" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="X17" s="12">
+        <v>10</v>
+      </c>
       <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
+      <c r="Z17" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
@@ -5265,23 +5778,23 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="5"/>
-        <v>column106</v>
+        <v>column104</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10016))::integer as column106</v>
+        <v>rpad(uniform(1,1234 , random(10016))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="8"/>
-        <v>column106::integer as column106</v>
+        <v>(case when uniform(1,1000,random(20016)) &gt; 300 then column104 else null end)::char(10) as column104</v>
       </c>
       <c r="J18">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K18">
         <f t="shared" si="10"/>
@@ -5289,11 +5802,11 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="11"/>
-        <v>integer</v>
-      </c>
-      <c r="M18" t="str">
+        <v>char</v>
+      </c>
+      <c r="M18">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="13"/>
@@ -5314,20 +5827,24 @@
         <v>48</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U18" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V18" s="12">
         <v>10000</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="X18" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X18" s="12">
+        <v>10</v>
+      </c>
       <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
+      <c r="Z18" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
       <c r="AC18" s="12"/>
@@ -5356,23 +5873,23 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="5"/>
-        <v>column107</v>
+        <v>column105</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10017))::double as column107</v>
+        <v>uniform(1,1234 , random(10017))::bigint as column105</v>
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="8"/>
-        <v>column107::double as column107</v>
+        <v>(case when uniform(1,1000,random(20017)) &gt; 300 then column105 else null end)::bigint as column105</v>
       </c>
       <c r="J19">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K19">
         <f t="shared" si="10"/>
@@ -5380,7 +5897,7 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="11"/>
-        <v>double</v>
+        <v>bigint</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="12"/>
@@ -5405,20 +5922,22 @@
         <v>48</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U19" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V19" s="12">
         <v>10000</v>
       </c>
       <c r="W19" s="12" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
+      <c r="Z19" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
@@ -5447,23 +5966,23 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="5"/>
-        <v>column108</v>
+        <v>column106</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10018))::float as column108</v>
+        <v>uniform(1,1234 , random(10018))::integer as column106</v>
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="8"/>
-        <v>column108::float as column108</v>
+        <v>(case when uniform(1,1000,random(20018)) &gt; 300 then column106 else null end)::integer as column106</v>
       </c>
       <c r="J20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K20">
         <f t="shared" si="10"/>
@@ -5471,7 +5990,7 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="11"/>
-        <v>float</v>
+        <v>integer</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="12"/>
@@ -5496,20 +6015,22 @@
         <v>48</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="U20" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V20" s="12">
         <v>10000</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
+      <c r="Z20" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
       <c r="AC20" s="12"/>
@@ -5538,23 +6059,23 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="5"/>
-        <v>column109</v>
+        <v>column107</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10019))::number(10,2) as column109</v>
+        <v>uniform(1,1234 , random(10019))::double as column107</v>
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="8"/>
-        <v>column109::number(10,2) as column109</v>
+        <v>(case when uniform(1,1000,random(20019)) &gt; 300 then column107 else null end)::double as column107</v>
       </c>
       <c r="J21">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K21">
         <f t="shared" si="10"/>
@@ -5562,15 +6083,15 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="11"/>
-        <v>number</v>
-      </c>
-      <c r="M21">
+        <v>double</v>
+      </c>
+      <c r="M21" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="N21">
+        <v/>
+      </c>
+      <c r="N21" t="str">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
@@ -5587,24 +6108,22 @@
         <v>48</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U21" s="12">
-        <v>100</v>
+        <v>1234</v>
       </c>
       <c r="V21" s="12">
         <v>10000</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X21" s="12">
-        <v>10</v>
-      </c>
-      <c r="Y21" s="12">
-        <v>2</v>
-      </c>
-      <c r="Z21" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
@@ -5629,27 +6148,27 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <v/>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="5"/>
-        <v>column110</v>
+        <v>column108</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column110</v>
+        <v>uniform(1,1234 , random(10020))::float as column108</v>
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="8"/>
-        <v>column110::integer as column110</v>
+        <v>(case when uniform(1,1000,random(20020)) &gt; 300 then column108 else null end)::float as column108</v>
       </c>
       <c r="J22">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K22">
         <f t="shared" si="10"/>
@@ -5657,7 +6176,7 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="11"/>
-        <v>integer</v>
+        <v>float</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="12"/>
@@ -5682,24 +6201,404 @@
         <v>48</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="U22" s="12">
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="V22" s="12">
         <v>10000</v>
       </c>
       <c r="W22" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
+      <c r="Z22" s="12">
+        <v>3000</v>
+      </c>
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="5"/>
+        <v>column109</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="6"/>
+        <v>uniform(1,1234 , random(10021))::number(10,2) as column109</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>1234</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="8"/>
+        <v>(case when uniform(1,1000,random(20021)) &gt; 300 then column109 else null end)::number(10,2) as column109</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="11"/>
+        <v>number</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="14"/>
+        <v>20021</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="15"/>
+        <v>10021</v>
+      </c>
+      <c r="R23" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="U23" s="12">
+        <v>1234</v>
+      </c>
+      <c r="V23" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X23" s="12">
+        <v>10</v>
+      </c>
+      <c r="Y23" s="12">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D24" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="5"/>
+        <v>column110</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="6"/>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="8"/>
+        <v>(case when uniform(1,1000,random(20022)) &gt; 300 then column110 else null end)::char(10) as column110</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="11"/>
+        <v>char</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O24">
+        <f t="shared" si="14"/>
+        <v>20022</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="15"/>
+        <v>10022</v>
+      </c>
+      <c r="R24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="U24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="V24" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W24" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X24" s="12">
+        <v>10</v>
+      </c>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12"/>
+      <c r="AD24" s="12"/>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D25" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="5"/>
+        <v>column111</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="6"/>
+        <v>seq8()::bigint as column111</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="7"/>
+        <v>10000</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="8"/>
+        <v>(case when uniform(1,1000,random(20023)) &gt; 300 then column111 else null end)::bigint as column111</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="11"/>
+        <v>bigint</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O25">
+        <f t="shared" si="14"/>
+        <v>20023</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="15"/>
+        <v>10023</v>
+      </c>
+      <c r="R25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T25" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="U25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="V25" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AD25" s="12"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D26" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="5"/>
+        <v>column112</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="6"/>
+        <v>null::integer as column112</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="8"/>
+        <v>(case when uniform(1,1000,random(20024)) &gt; 300 then column112 else null end)::integer as column112</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="11"/>
+        <v>integer</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O26">
+        <f t="shared" si="14"/>
+        <v>20024</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="15"/>
+        <v>10024</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T26" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U26" s="12">
+        <v>0</v>
+      </c>
+      <c r="V26" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AD177" xr:uid="{1DEE4BB0-2492-0346-9743-0CF6D1D58AA5}"/>
@@ -5711,8 +6610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AC2046-8798-C848-AA97-D3B5154A7925}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5889,12 +6788,13 @@
 IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L3,
+""))))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -5912,7 +6812,7 @@
         <v>normal::bigint as normal</v>
       </c>
       <c r="J3">
-        <f>IF((Z3=0),0,INT((Z3/V3)*1000))</f>
+        <f>IF(ISBLANK(Z3),0,IF(TRIM(Z3)="",0,INT((Z3/V3)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K3">
@@ -5963,7 +6863,9 @@
       </c>
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
+      <c r="Z3" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AA3" s="12">
         <v>1</v>
       </c>
@@ -6005,12 +6907,13 @@
 IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-"")))))))))),"::",L4,
+""))))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -6028,7 +6931,7 @@
         <v>normal::char(6) as normal</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J7" si="9">IF((Z4=0),0,INT((Z4/V4)*1000))</f>
+        <f t="shared" ref="J4:J7" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K4">
@@ -6081,7 +6984,9 @@
         <v>6</v>
       </c>
       <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="Z4" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="AA4" s="12">
         <v>1</v>
       </c>
@@ -6182,7 +7087,9 @@
         <v>6</v>
       </c>
       <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
+      <c r="Z5" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AA5" s="12">
         <v>1</v>
       </c>
@@ -6283,7 +7190,9 @@
         <v>6</v>
       </c>
       <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
+      <c r="Z6" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12" t="s">
         <v>10</v>
@@ -6380,7 +7289,9 @@
       </c>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="Z7" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12" t="s">
         <v>10</v>
@@ -6404,294 +7315,294 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
varchar with variable length caused a problem with the number of unique values. Therefor, CHAR and VARCHAR will be handled the same way
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE6CC5A0-2342-8644-B746-5E58200F79AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23B21CFE-E912-9F45-B49A-F92F4160B851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="4" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="2" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -1138,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2F4A9-4178-7746-B810-92567ADD6A96}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1922,10 +1922,10 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3:Z26"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2095,16 +2095,14 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L3,
+IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -2195,16 +2193,14 @@
         <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L4,
+IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -2293,7 +2289,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10003))::varchar,uniform(length(1234),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>rpad(uniform(1,1234 , random(10003))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
@@ -3319,7 +3315,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10015))::varchar,uniform(length(1234),10,random(10015+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>rpad(uniform(1,1234 , random(10015))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -4161,11 +4157,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD38527B-8DA9-F048-9888-D8112A4B2F49}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4345,16 +4341,14 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L3,
+IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -4456,16 +4450,14 @@
         <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L4,
+IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -4565,7 +4557,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10003))::varchar,uniform(length(1234),10,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>rpad(uniform(1,1234 , random(10003))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
@@ -5687,7 +5679,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10015))::varchar,uniform(length(1234),10,random(10015+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>rpad(uniform(1,1234 , random(10015))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -6610,8 +6602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AC2046-8798-C848-AA97-D3B5154A7925}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6785,16 +6777,14 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(L3="VARCHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L3="CHAR",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L3="varchar",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,uniform(length(",H3,"),",M3,",random(",P3,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L3,
+IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -6901,65 +6891,63 @@
         <v>normal</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G7" si="6">_xlfn.CONCAT(
+        <f>_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(L4="VARCHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L4="CHAR",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L4="varchar",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,uniform(length(",H4,"),",M4,",random(",P4,"+20000)),'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))))),"::",L4,
+IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>rpad(abs(trunc((5+normal(0,1,random(10002)))*(100/20)))::varchar,6,'abcdefghifklmnopqrstuvwxyz')::char(6) as normal</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H7" si="7">U4</f>
+        <f t="shared" ref="H4:H7" si="6">U4</f>
         <v>100</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I7" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
+        <f t="shared" ref="I4:I7" si="7">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>normal::char(6) as normal</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J7" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
+        <f t="shared" ref="J4:J7" si="8">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K7" si="10">V4</f>
+        <f t="shared" ref="K4:K7" si="9">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L7" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
+        <f t="shared" ref="L4:L7" si="10">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
         <v>char</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M7" si="12">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M7" si="11">IF(ISBLANK(X4),"",X4)</f>
         <v>6</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N7" si="13">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N7" si="12">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O7" si="14">O3+1</f>
+        <f t="shared" ref="O4:O7" si="13">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P7" si="15">P3+1</f>
+        <f t="shared" ref="P4:P7" si="14">P3+1</f>
         <v>10002</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q7" si="16">AA4</f>
+        <f t="shared" ref="Q4:Q7" si="15">AA4</f>
         <v>1</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -7022,47 +7010,60 @@
         <v>normal</v>
       </c>
       <c r="G5" t="str">
+        <f t="shared" ref="G5:G7" si="16">_xlfn.CONCAT(
+IF(H5=0,"null",
+IF(AND(L5="bigint",Q5=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P5,")))*(",H5,"/20)))"),
+IF(AND(OR(L5="char",L5="varchar"),Q5=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P5,")))*(",H5,"/20)))::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L5="bigint",H5=K5),"seq8()",
+IF(AND(OR(L5="char",L5="varchar"),H5=K5),_xlfn.CONCAT("rpad(seq8()::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L5="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H5," , random(",P5,")),current_date)"),
+IF(OR(OR(OR(OR(L5="bigint",L5="double"),L5="integer"),L5="number"),L5="float"),_xlfn.CONCAT("uniform(1,",H5," , random(",P5,"))"),
+IF(L5="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H5,", random(",P5,"))))"),
+IF(OR(L5="char",L5="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H5," , random(",P5,"))::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
+""))))))))),"::",L5,
+IF(OR(L5="varchar",L5="char"),_xlfn.CONCAT("(",M5,")"),
+IF(L5="number",_xlfn.CONCAT("(",M5,",",N5,")"),"")),
+" as ",F5)</f>
+        <v>rpad(abs(trunc((5+normal(0,1,random(10003)))*(100/20)))::varchar,6,'abcdefghifklmnopqrstuvwxyz')::varchar(6) as normal</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="6"/>
-        <v>rpad(abs(trunc((5+normal(0,1,random(10003)))*(100/20)))::varchar,uniform(length(100),6,random(10003+20000)),'abcdefghifklmnopqrstuvwxyz')::varchar(6) as normal</v>
-      </c>
-      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="I5" t="str">
+        <v>normal::varchar(6) as normal</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="8"/>
-        <v>normal::varchar(6) as normal</v>
-      </c>
-      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K5">
+        <v>10000</v>
+      </c>
+      <c r="L5" t="str">
         <f t="shared" si="10"/>
-        <v>10000</v>
-      </c>
-      <c r="L5" t="str">
+        <v>varchar</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="11"/>
-        <v>varchar</v>
-      </c>
-      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="12"/>
-        <v>6</v>
-      </c>
-      <c r="N5" t="str">
+        <v/>
+      </c>
+      <c r="O5">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="O5">
+        <v>20003</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="14"/>
-        <v>20003</v>
-      </c>
-      <c r="P5">
+        <v>10003</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="15"/>
-        <v>10003</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="R5" s="12" t="s">
@@ -7125,47 +7126,47 @@
         <v>uniform</v>
       </c>
       <c r="G6" t="str">
+        <f t="shared" si="16"/>
+        <v>uniform(1,100 , random(10004))::bigint as uniform</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="6"/>
-        <v>uniform(1,100 , random(10004))::bigint as uniform</v>
-      </c>
-      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="7"/>
-        <v>100</v>
-      </c>
-      <c r="I6" t="str">
+        <v>uniform::bigint as uniform</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="8"/>
-        <v>uniform::bigint as uniform</v>
-      </c>
-      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K6">
+        <v>10000</v>
+      </c>
+      <c r="L6" t="str">
         <f t="shared" si="10"/>
-        <v>10000</v>
-      </c>
-      <c r="L6" t="str">
+        <v>bigint</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="12"/>
-        <v>6</v>
-      </c>
-      <c r="N6" t="str">
+        <v/>
+      </c>
+      <c r="O6">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="O6">
+        <v>20004</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="14"/>
-        <v>20004</v>
-      </c>
-      <c r="P6">
+        <v>10004</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="15"/>
-        <v>10004</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R6" s="12" t="s">
@@ -7226,47 +7227,47 @@
         <v>id</v>
       </c>
       <c r="G7" t="str">
+        <f t="shared" si="16"/>
+        <v>seq8()::bigint as id</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="6"/>
-        <v>seq8()::bigint as id</v>
-      </c>
-      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" si="7"/>
+        <v>id::bigint as id</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" si="8"/>
-        <v>id::bigint as id</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K7">
+      <c r="L7" t="str">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="L7" t="str">
+        <v>bigint</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="N7" t="str">
+      <c r="O7">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="O7">
+        <v>20005</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="14"/>
-        <v>20005</v>
-      </c>
-      <c r="P7">
+        <v>10005</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="15"/>
-        <v>10005</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R7" s="12" t="s">

</xml_diff>

<commit_message>
added logic for randstr for varchar
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23B21CFE-E912-9F45-B49A-F92F4160B851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F4816A-9CB5-2F40-8788-65DD78C8F636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="2" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -29,12 +29,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="85">
   <si>
     <t>TableName</t>
   </si>
@@ -795,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0D2BAD-D4C8-E14C-84C0-77F87BA6FA10}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:M8"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1138,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2F4A9-4178-7746-B810-92567ADD6A96}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1921,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
@@ -1935,7 +1941,7 @@
     <col min="4" max="4" width="85.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="145.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="130.83203125" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
@@ -2095,14 +2101,15 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L3,
+IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L3="varchar",_xlfn.CONCAT("randstr(uniform(1,",M3,", random(",P3,")),uniform(1,",H3,",random(",P3,")))"),
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -2193,14 +2200,15 @@
         <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L4,
+IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L4="varchar",_xlfn.CONCAT("randstr(uniform(1,",M4,", random(",P4,")),uniform(1,",H4,",random(",P4,")))"),
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -2289,7 +2297,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10003))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>randstr(uniform(1,10, random(10003)),uniform(1,1234,random(10003)))::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
@@ -3315,7 +3323,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10015))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>randstr(uniform(1,10, random(10015)),uniform(1,1234,random(10015)))::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -4158,7 +4166,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
@@ -4341,14 +4349,15 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L3,
+IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L3="varchar",_xlfn.CONCAT("randstr(uniform(1,",M3,", random(",P3,")),uniform(1,",H3,",random(",P3,")))"),
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -4450,14 +4459,15 @@
         <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L4,
+IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L4="varchar",_xlfn.CONCAT("randstr(uniform(1,",M4,", random(",P4,")),uniform(1,",H4,",random(",P4,")))"),
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
@@ -4557,7 +4567,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10003))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column3</v>
+        <v>randstr(uniform(1,10, random(10003)),uniform(1,1234,random(10003)))::varchar(10) as column3</v>
       </c>
       <c r="H5">
         <f t="shared" si="7"/>
@@ -5679,7 +5689,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10015))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::varchar(10) as column103</v>
+        <v>randstr(uniform(1,10, random(10015)),uniform(1,1234,random(10015)))::varchar(10) as column103</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -6600,10 +6610,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AC2046-8798-C848-AA97-D3B5154A7925}">
-  <dimension ref="A1:AD7"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6613,7 +6623,7 @@
     <col min="4" max="4" width="85.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.5" customWidth="1"/>
     <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.5" customWidth="1"/>
+    <col min="7" max="7" width="91" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
@@ -6777,14 +6787,15 @@
         <f>_xlfn.CONCAT(
 IF(H3=0,"null",
 IF(AND(L3="bigint",Q3=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))"),
-IF(AND(OR(L3="char",L3="varchar"),Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",Q3=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P3,")))*(",H3,"/20)))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L3="bigint",H3=K3),"seq8()",
-IF(AND(OR(L3="char",L3="varchar"),H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
-IF(OR(L3="char",L3="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L3,
+IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L3="varchar",_xlfn.CONCAT("randstr(uniform(1,",M3,", random(",P3,")),uniform(1,",H3,",random(",P3,")))"),
+"")))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -6867,87 +6878,88 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4">
-        <f t="shared" ref="A4:A7" si="0">A3+1</f>
+        <f t="shared" ref="A4:A6" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B7" si="1">R4</f>
+        <f t="shared" ref="B4:B6" si="1">R4</f>
         <v>dbo</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C7" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C6" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>child</v>
       </c>
       <c r="D4" s="4" t="str">
-        <f t="shared" ref="D4:D7" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
+        <f t="shared" ref="D4:D6" si="3">IF(C3=C4,"",_xlfn.CONCAT("create transient schema if not exists ",B4," data_retention_time_in_days=0;  create or replace table ",B4,".",C4," as select"))</f>
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E7" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <f t="shared" ref="E4:E6" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
         <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F7" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <f t="shared" ref="F4:F6" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
         <v>normal</v>
       </c>
       <c r="G4" t="str">
-        <f>_xlfn.CONCAT(
+        <f t="shared" ref="G4:G6" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
-IF(AND(OR(L4="char",L4="varchar"),Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
-IF(AND(OR(L4="char",L4="varchar"),H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
-IF(OR(L4="char",L4="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L4,
+IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
+IF(L4="varchar",_xlfn.CONCAT("randstr(uniform(1,",M4,", random(",P4,")),uniform(1,",H4,",random(",P4,")))"),
+"")))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>rpad(abs(trunc((5+normal(0,1,random(10002)))*(100/20)))::varchar,6,'abcdefghifklmnopqrstuvwxyz')::char(6) as normal</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H7" si="6">U4</f>
+        <f t="shared" ref="H4:H6" si="7">U4</f>
         <v>100</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I7" si="7">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
+        <f t="shared" ref="I4:I6" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>normal::char(6) as normal</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J7" si="8">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
+        <f t="shared" ref="J4:J6" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K7" si="9">V4</f>
+        <f t="shared" ref="K4:K6" si="10">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L7" si="10">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
+        <f t="shared" ref="L4:L6" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
         <v>char</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M7" si="11">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M6" si="12">IF(ISBLANK(X4),"",X4)</f>
         <v>6</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N7" si="12">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N6" si="13">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O7" si="13">O3+1</f>
+        <f t="shared" ref="O4:O6" si="14">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P7" si="14">P3+1</f>
+        <f t="shared" ref="P4:P6" si="15">P3+1</f>
         <v>10002</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q7" si="15">AA4</f>
+        <f t="shared" ref="Q4:Q6" si="16">AA4</f>
         <v>1</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -7003,68 +7015,55 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="5"/>
-        <v>normal</v>
+        <v>uniform</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" ref="G5:G7" si="16">_xlfn.CONCAT(
-IF(H5=0,"null",
-IF(AND(L5="bigint",Q5=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P5,")))*(",H5,"/20)))"),
-IF(AND(OR(L5="char",L5="varchar"),Q5=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P5,")))*(",H5,"/20)))::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(AND(L5="bigint",H5=K5),"seq8()",
-IF(AND(OR(L5="char",L5="varchar"),H5=K5),_xlfn.CONCAT("rpad(seq8()::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
-IF(L5="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H5," , random(",P5,")),current_date)"),
-IF(OR(OR(OR(OR(L5="bigint",L5="double"),L5="integer"),L5="number"),L5="float"),_xlfn.CONCAT("uniform(1,",H5," , random(",P5,"))"),
-IF(L5="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H5,", random(",P5,"))))"),
-IF(OR(L5="char",L5="varchar"),_xlfn.CONCAT("rpad(uniform(1,",H5," , random(",P5,"))::varchar,",M5,",'abcdefghifklmnopqrstuvwxyz')"),
-""))))))))),"::",L5,
-IF(OR(L5="varchar",L5="char"),_xlfn.CONCAT("(",M5,")"),
-IF(L5="number",_xlfn.CONCAT("(",M5,",",N5,")"),"")),
-" as ",F5)</f>
-        <v>rpad(abs(trunc((5+normal(0,1,random(10003)))*(100/20)))::varchar,6,'abcdefghifklmnopqrstuvwxyz')::varchar(6) as normal</v>
+        <f t="shared" si="6"/>
+        <v>uniform(1,100 , random(10003))::bigint as uniform</v>
       </c>
       <c r="H5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="7"/>
-        <v>normal::varchar(6) as normal</v>
+        <f t="shared" si="8"/>
+        <v>uniform::bigint as uniform</v>
       </c>
       <c r="J5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10000</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="10"/>
-        <v>varchar</v>
+        <f t="shared" si="11"/>
+        <v>bigint</v>
       </c>
       <c r="M5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="O5">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>20003</v>
       </c>
       <c r="P5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>10003</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <f t="shared" si="16"/>
+        <v>0</v>
       </c>
       <c r="R5" s="12" t="s">
         <v>12</v>
@@ -7073,7 +7072,7 @@
         <v>36</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U5" s="12">
         <v>100</v>
@@ -7082,7 +7081,7 @@
         <v>10000</v>
       </c>
       <c r="W5" s="12" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="X5" s="12">
         <v>6</v>
@@ -7091,9 +7090,7 @@
       <c r="Z5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AA5" s="12">
-        <v>1</v>
-      </c>
+      <c r="AA5" s="12"/>
       <c r="AB5" s="12" t="s">
         <v>10</v>
       </c>
@@ -7111,88 +7108,86 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="2"/>
-        <v>child</v>
+        <v>parent</v>
       </c>
       <c r="D6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.parent as select</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <v>from table(generator(rowcount =&gt; 100))</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="5"/>
-        <v>uniform</v>
+        <v>id</v>
       </c>
       <c r="G6" t="str">
+        <f t="shared" si="6"/>
+        <v>seq8()::bigint as id</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="8"/>
+        <v>id::bigint as id</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="11"/>
+        <v>bigint</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O6">
+        <f t="shared" si="14"/>
+        <v>20004</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="15"/>
+        <v>10004</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="16"/>
-        <v>uniform(1,100 , random(10004))::bigint as uniform</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="7"/>
-        <v>uniform::bigint as uniform</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="9"/>
-        <v>10000</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="10"/>
-        <v>bigint</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="11"/>
-        <v>6</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="O6">
-        <f t="shared" si="13"/>
-        <v>20004</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="14"/>
-        <v>10004</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="R6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="U6" s="12">
         <v>100</v>
       </c>
       <c r="V6" s="12">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="W6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="12">
-        <v>6</v>
-      </c>
+      <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12" t="s">
@@ -7200,105 +7195,6 @@
       </c>
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="1"/>
-        <v>dbo</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="2"/>
-        <v>parent</v>
-      </c>
-      <c r="D7" s="4" t="str">
-        <f t="shared" si="3"/>
-        <v>create transient schema if not exists dbo data_retention_time_in_days=0;  create or replace table dbo.parent as select</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 100))</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="5"/>
-        <v>id</v>
-      </c>
-      <c r="G7" t="str">
-        <f t="shared" si="16"/>
-        <v>seq8()::bigint as id</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="7"/>
-        <v>id::bigint as id</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="9"/>
-        <v>100</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="10"/>
-        <v>bigint</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="O7">
-        <f t="shared" si="13"/>
-        <v>20005</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="14"/>
-        <v>10005</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" s="12">
-        <v>100</v>
-      </c>
-      <c r="V7" s="12">
-        <v>100</v>
-      </c>
-      <c r="W7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC7" s="12"/>
-      <c r="AD7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added support for datatype BOOLEAN
</commit_message>
<xml_diff>
--- a/datageneration_sample_spreadsheet.xlsx
+++ b/datageneration_sample_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfehrmann/fehrminator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F4816A-9CB5-2F40-8788-65DD78C8F636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C44B05-223B-0F45-AAEF-FA0F0B0BE1B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="3" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
+    <workbookView xWindow="920" yWindow="640" windowWidth="27400" windowHeight="16220" activeTab="4" xr2:uid="{29A8BBA8-8134-DE49-96D2-ABB6257BC38C}"/>
   </bookViews>
   <sheets>
     <sheet name="Spec" sheetId="11" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="assemble.awk " sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'NULL Values Example'!$A$1:$AD$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'NULL Values Example'!$A$1:$AD$179</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="88">
   <si>
     <t>TableName</t>
   </si>
@@ -323,6 +325,15 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>column13</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>column113</t>
   </si>
 </sst>
 </file>
@@ -445,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -476,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -801,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0D2BAD-D4C8-E14C-84C0-77F87BA6FA10}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:M16"/>
     </sheetView>
   </sheetViews>
@@ -822,51 +834,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
@@ -910,149 +922,149 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" ht="34" customHeight="1">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="34" customHeight="1">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" ht="34" customHeight="1">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13" ht="34" customHeight="1">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:13" ht="34" customHeight="1">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="14" spans="1:13" ht="34" customHeight="1">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:13" ht="34" customHeight="1">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" ht="34" customHeight="1">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1142,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB2F4A9-4178-7746-B810-92567ADD6A96}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1542,13 +1554,13 @@
         <v>81</v>
       </c>
       <c r="D14" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14" s="12">
         <v>10000</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1568,22 +1580,20 @@
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D15" s="12">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="E15" s="12">
         <v>10000</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
-      <c r="I15" s="12">
-        <v>3000</v>
-      </c>
+      <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -1597,7 +1607,7 @@
         <v>48</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="12">
         <v>1234</v>
@@ -1606,7 +1616,7 @@
         <v>10000</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
@@ -1626,7 +1636,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="12">
         <v>1234</v>
@@ -1635,11 +1645,9 @@
         <v>10000</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12">
         <v>3000</v>
@@ -1657,7 +1665,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="12">
         <v>1234</v>
@@ -1666,7 +1674,7 @@
         <v>10000</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G18" s="12">
         <v>10</v>
@@ -1688,7 +1696,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D19" s="12">
         <v>1234</v>
@@ -1697,9 +1705,11 @@
         <v>10000</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="G19" s="12">
+        <v>10</v>
+      </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12">
         <v>3000</v>
@@ -1717,7 +1727,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="12">
         <v>1234</v>
@@ -1726,7 +1736,7 @@
         <v>10000</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
@@ -1746,7 +1756,7 @@
         <v>48</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="12">
         <v>1234</v>
@@ -1755,7 +1765,7 @@
         <v>10000</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
@@ -1775,7 +1785,7 @@
         <v>48</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" s="12">
         <v>1234</v>
@@ -1784,7 +1794,7 @@
         <v>10000</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -1804,7 +1814,7 @@
         <v>48</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="12">
         <v>1234</v>
@@ -1813,14 +1823,10 @@
         <v>10000</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="12">
-        <v>10</v>
-      </c>
-      <c r="H23" s="12">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="12">
         <v>3000</v>
       </c>
@@ -1837,21 +1843,23 @@
         <v>48</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="12">
-        <v>10000</v>
+        <v>1234</v>
       </c>
       <c r="E24" s="12">
         <v>10000</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G24" s="12">
         <v>10</v>
       </c>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12">
+        <v>2</v>
+      </c>
       <c r="I24" s="12">
         <v>3000</v>
       </c>
@@ -1868,7 +1876,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D25" s="12">
         <v>10000</v>
@@ -1877,9 +1885,11 @@
         <v>10000</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="G25" s="12">
+        <v>10</v>
+      </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12">
         <v>3000</v>
@@ -1897,16 +1907,16 @@
         <v>48</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E26" s="12">
         <v>10000</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
@@ -1917,6 +1927,64 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="12">
+        <v>2</v>
+      </c>
+      <c r="E27" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="12">
+        <v>0</v>
+      </c>
+      <c r="E28" s="12">
+        <v>10000</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12">
+        <v>3000</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1925,13 +1993,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91D98FF-FC92-6248-BA4C-8B2D1A166A29}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
+      <selection pane="bottomRight" activeCell="O25" sqref="O25:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2105,11 +2173,12 @@
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
+IF(L3="boolean",_xlfn.CONCAT("(uniform(1,",H3,",random(",P3,"))-1)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("randstr(uniform(1,",M3,", random(",P3,")),uniform(1,",H3,",random(",P3,")))"),
-"")))))))))),"::",L3,
+""))))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -2177,11 +2246,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B26" si="1">R4</f>
+        <f t="shared" ref="B4:B28" si="1">R4</f>
         <v>schema1</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C26" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C28" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
@@ -2189,57 +2258,58 @@
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E26" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <f t="shared" ref="E4:E28" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
         <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F26" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <f t="shared" ref="F4:F28" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
         <v>column2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
+        <f t="shared" ref="G4:G28" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
 IF(AND(L4="char",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
+IF(L4="boolean",_xlfn.CONCAT("(uniform(1,",H4,",random(",P4,"))-1)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("randstr(uniform(1,",M4,", random(",P4,")),uniform(1,",H4,",random(",P4,")))"),
-"")))))))))),"::",L4,
+""))))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10002))))::timestamp as column2</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H26" si="7">U4</f>
+        <f t="shared" ref="H4:H28" si="7">U4</f>
         <v>1234</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K26" si="8">V4</f>
+        <f t="shared" ref="K4:K28" si="8">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L26" si="9">W4</f>
+        <f t="shared" ref="L4:L28" si="9">W4</f>
         <v>timestamp</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M26" si="10">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M28" si="10">IF(ISBLANK(X4),"",X4)</f>
         <v/>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N26" si="11">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N28" si="11">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O26" si="12">O3+1</f>
+        <f t="shared" ref="O4:O28" si="12">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P26" si="13">P3+1</f>
+        <f t="shared" ref="P4:P28" si="13">P3+1</f>
         <v>10002</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -3043,19 +3113,19 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>A12+1</f>
+        <v>11</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B14" si="14">R14</f>
         <v>schema1</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C14" si="15">_xlfn.CONCAT($C$2,S14,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C12=C14,"",_xlfn.CONCAT("create transient schema if not exists ",B14," data_retention_time_in_days=0;  create or replace table ",B14,".",C14," as select"))</f>
         <v/>
       </c>
       <c r="E14" t="str">
@@ -3063,31 +3133,31 @@
         <v/>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F14" si="16">_xlfn.CONCAT($F$2,T14,$F$2)</f>
         <v>column12</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column12</v>
+        <v>(uniform(1,2,random(10012))-1)::boolean as column12</v>
       </c>
       <c r="H14">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" ref="H14" si="17">U14</f>
+        <v>2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K14" si="18">V14</f>
         <v>10000</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="9"/>
-        <v>integer</v>
+        <f t="shared" ref="L14" si="19">W14</f>
+        <v>boolean</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="M14" si="20">IF(ISBLANK(X14),"",X14)</f>
         <v/>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N14" si="21">IF(ISBLANK(Y14),"",Y14)</f>
         <v/>
       </c>
       <c r="O14">
@@ -3108,13 +3178,13 @@
         <v>81</v>
       </c>
       <c r="U14" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="12">
         <v>10000</v>
       </c>
       <c r="W14" s="12" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
@@ -3128,8 +3198,8 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>A13+1</f>
+        <v>12</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
@@ -3140,7 +3210,7 @@
         <v>table1</v>
       </c>
       <c r="D15" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C13=C15,"",_xlfn.CONCAT("create transient schema if not exists ",B15," data_retention_time_in_days=0;  create or replace table ",B15,".",C15," as select"))</f>
         <v/>
       </c>
       <c r="E15" t="str">
@@ -3149,15 +3219,15 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="5"/>
-        <v>column101</v>
+        <v>column13</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="6"/>
-        <v>dateadd(day,uniform(1,1234 , random(10013)),current_date)::date as column101</v>
+        <v>null::integer as column13</v>
       </c>
       <c r="H15">
         <f t="shared" si="7"/>
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="8"/>
@@ -3165,7 +3235,7 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="9"/>
-        <v>date</v>
+        <v>integer</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="10"/>
@@ -3190,21 +3260,21 @@
         <v>48</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="U15" s="12">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="V15" s="12">
         <v>10000</v>
       </c>
       <c r="W15" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="12">
-        <v>3000</v>
+      <c r="Z15" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
@@ -3214,7 +3284,7 @@
     <row r="16" spans="1:30">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
@@ -3234,11 +3304,11 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="5"/>
-        <v>column102</v>
+        <v>column101</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10014))))::timestamp as column102</v>
+        <v>dateadd(day,uniform(1,1234 , random(10014)),current_date)::date as column101</v>
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
@@ -3250,7 +3320,7 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="9"/>
-        <v>timestamp</v>
+        <v>date</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="10"/>
@@ -3275,7 +3345,7 @@
         <v>48</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U16" s="12">
         <v>1234</v>
@@ -3284,7 +3354,7 @@
         <v>10000</v>
       </c>
       <c r="W16" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -3299,7 +3369,7 @@
     <row r="17" spans="1:30">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
@@ -3319,11 +3389,11 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="5"/>
-        <v>column103</v>
+        <v>column102</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>randstr(uniform(1,10, random(10015)),uniform(1,1234,random(10015)))::varchar(10) as column103</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10015))))::timestamp as column102</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -3335,11 +3405,11 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="9"/>
-        <v>varchar</v>
-      </c>
-      <c r="M17">
+        <v>timestamp</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="11"/>
@@ -3360,7 +3430,7 @@
         <v>48</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U17" s="12">
         <v>1234</v>
@@ -3369,11 +3439,9 @@
         <v>10000</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X17" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12">
         <v>3000</v>
@@ -3386,7 +3454,7 @@
     <row r="18" spans="1:30">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="1"/>
@@ -3406,11 +3474,11 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="5"/>
-        <v>column104</v>
+        <v>column103</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10016))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
+        <v>randstr(uniform(1,10, random(10016)),uniform(1,1234,random(10016)))::varchar(10) as column103</v>
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
@@ -3422,7 +3490,7 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="9"/>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="M18">
         <f t="shared" si="10"/>
@@ -3447,7 +3515,7 @@
         <v>48</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U18" s="12">
         <v>1234</v>
@@ -3456,7 +3524,7 @@
         <v>10000</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X18" s="12">
         <v>10</v>
@@ -3473,7 +3541,7 @@
     <row r="19" spans="1:30">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="1"/>
@@ -3493,11 +3561,11 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="5"/>
-        <v>column105</v>
+        <v>column104</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10017))::bigint as column105</v>
+        <v>rpad(uniform(1,1234 , random(10017))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
@@ -3509,11 +3577,11 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="9"/>
-        <v>bigint</v>
-      </c>
-      <c r="M19" t="str">
+        <v>char</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="10"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="11"/>
@@ -3534,7 +3602,7 @@
         <v>48</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U19" s="12">
         <v>1234</v>
@@ -3543,9 +3611,11 @@
         <v>10000</v>
       </c>
       <c r="W19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X19" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X19" s="12">
+        <v>10</v>
+      </c>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12">
         <v>3000</v>
@@ -3558,7 +3628,7 @@
     <row r="20" spans="1:30">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
@@ -3578,11 +3648,11 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="5"/>
-        <v>column106</v>
+        <v>column105</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10018))::integer as column106</v>
+        <v>uniform(1,1234 , random(10018))::bigint as column105</v>
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
@@ -3594,7 +3664,7 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="9"/>
-        <v>integer</v>
+        <v>bigint</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="10"/>
@@ -3619,7 +3689,7 @@
         <v>48</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U20" s="12">
         <v>1234</v>
@@ -3628,7 +3698,7 @@
         <v>10000</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
@@ -3643,7 +3713,7 @@
     <row r="21" spans="1:30">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="1"/>
@@ -3663,11 +3733,11 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="5"/>
-        <v>column107</v>
+        <v>column106</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10019))::double as column107</v>
+        <v>uniform(1,1234 , random(10019))::integer as column106</v>
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
@@ -3679,7 +3749,7 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="9"/>
-        <v>double</v>
+        <v>integer</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="10"/>
@@ -3704,7 +3774,7 @@
         <v>48</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U21" s="12">
         <v>1234</v>
@@ -3713,7 +3783,7 @@
         <v>10000</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
@@ -3728,7 +3798,7 @@
     <row r="22" spans="1:30">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="1"/>
@@ -3748,11 +3818,11 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="5"/>
-        <v>column108</v>
+        <v>column107</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10020))::float as column108</v>
+        <v>uniform(1,1234 , random(10020))::double as column107</v>
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
@@ -3764,7 +3834,7 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="9"/>
-        <v>float</v>
+        <v>double</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="10"/>
@@ -3789,7 +3859,7 @@
         <v>48</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U22" s="12">
         <v>1234</v>
@@ -3798,7 +3868,7 @@
         <v>10000</v>
       </c>
       <c r="W22" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
@@ -3813,7 +3883,7 @@
     <row r="23" spans="1:30">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
@@ -3833,11 +3903,11 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="5"/>
-        <v>column109</v>
+        <v>column108</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10021))::number(10,2) as column109</v>
+        <v>uniform(1,1234 , random(10021))::float as column108</v>
       </c>
       <c r="H23">
         <f t="shared" si="7"/>
@@ -3849,15 +3919,15 @@
       </c>
       <c r="L23" t="str">
         <f t="shared" si="9"/>
-        <v>number</v>
-      </c>
-      <c r="M23">
+        <v>float</v>
+      </c>
+      <c r="M23" t="str">
         <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="N23">
+        <v/>
+      </c>
+      <c r="N23" t="str">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="O23">
         <f t="shared" si="12"/>
@@ -3874,7 +3944,7 @@
         <v>48</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U23" s="12">
         <v>1234</v>
@@ -3883,14 +3953,10 @@
         <v>10000</v>
       </c>
       <c r="W23" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X23" s="12">
-        <v>10</v>
-      </c>
-      <c r="Y23" s="12">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
       <c r="Z23" s="12">
         <v>3000</v>
       </c>
@@ -3902,7 +3968,7 @@
     <row r="24" spans="1:30">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="1"/>
@@ -3922,15 +3988,15 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="5"/>
-        <v>column110</v>
+        <v>column109</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
+        <v>uniform(1,1234 , random(10022))::number(10,2) as column109</v>
       </c>
       <c r="H24">
         <f t="shared" si="7"/>
-        <v>10000</v>
+        <v>1234</v>
       </c>
       <c r="K24">
         <f t="shared" si="8"/>
@@ -3938,15 +4004,15 @@
       </c>
       <c r="L24" t="str">
         <f t="shared" si="9"/>
-        <v>char</v>
+        <v>number</v>
       </c>
       <c r="M24">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="N24" t="str">
+      <c r="N24">
         <f t="shared" si="11"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="O24">
         <f t="shared" si="12"/>
@@ -3956,28 +4022,30 @@
         <f t="shared" si="13"/>
         <v>10022</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="12" t="s">
         <v>47</v>
       </c>
       <c r="S24" s="12" t="s">
         <v>48</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U24" s="12">
-        <v>10000</v>
+        <v>1234</v>
       </c>
       <c r="V24" s="12">
         <v>10000</v>
       </c>
       <c r="W24" s="12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="X24" s="12">
         <v>10</v>
       </c>
-      <c r="Y24" s="12"/>
+      <c r="Y24" s="12">
+        <v>2</v>
+      </c>
       <c r="Z24" s="12">
         <v>3000</v>
       </c>
@@ -3989,7 +4057,7 @@
     <row r="25" spans="1:30">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="1"/>
@@ -4009,11 +4077,11 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="5"/>
-        <v>column111</v>
+        <v>column110</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="6"/>
-        <v>seq8()::bigint as column111</v>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
       </c>
       <c r="H25">
         <f t="shared" si="7"/>
@@ -4025,11 +4093,11 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="9"/>
-        <v>bigint</v>
-      </c>
-      <c r="M25" t="str">
+        <v>char</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="10"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="11"/>
@@ -4043,14 +4111,14 @@
         <f t="shared" si="13"/>
         <v>10023</v>
       </c>
-      <c r="R25" s="12" t="s">
+      <c r="R25" s="13" t="s">
         <v>47</v>
       </c>
       <c r="S25" s="12" t="s">
         <v>48</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="U25" s="12">
         <v>10000</v>
@@ -4058,10 +4126,12 @@
       <c r="V25" s="12">
         <v>10000</v>
       </c>
-      <c r="W25" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="X25" s="12"/>
+      <c r="W25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X25" s="12">
+        <v>10</v>
+      </c>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12">
         <v>3000</v>
@@ -4074,7 +4144,7 @@
     <row r="26" spans="1:30">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="1"/>
@@ -4090,19 +4160,19 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <v/>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="5"/>
-        <v>column112</v>
+        <v>column111</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column112</v>
+        <v>seq8()::bigint as column111</v>
       </c>
       <c r="H26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="K26">
         <f t="shared" si="8"/>
@@ -4110,7 +4180,7 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="9"/>
-        <v>integer</v>
+        <v>bigint</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="10"/>
@@ -4135,16 +4205,16 @@
         <v>48</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U26" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V26" s="12">
         <v>10000</v>
       </c>
-      <c r="W26" s="12" t="s">
-        <v>59</v>
+      <c r="W26" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
@@ -4155,6 +4225,176 @@
       <c r="AB26" s="12"/>
       <c r="AC26" s="12"/>
       <c r="AD26" s="12"/>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27">
+        <f>A25+1</f>
+        <v>23</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ref="B27" si="22">R27</f>
+        <v>schema1</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ref="C27" si="23">_xlfn.CONCAT($C$2,S27,$C$2)</f>
+        <v>table1</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <f>IF(C25=C27,"",_xlfn.CONCAT("create transient schema if not exists ",B27," data_retention_time_in_days=0;  create or replace table ",B27,".",C27," as select"))</f>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" ref="F27" si="24">_xlfn.CONCAT($F$2,T27,$F$2)</f>
+        <v>column112</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="6"/>
+        <v>(uniform(1,2,random(10025))-1)::boolean as column112</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27" si="25">U27</f>
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27" si="26">V27</f>
+        <v>10000</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" ref="L27" si="27">W27</f>
+        <v>boolean</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" ref="M27" si="28">IF(ISBLANK(X27),"",X27)</f>
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" ref="N27" si="29">IF(ISBLANK(Y27),"",Y27)</f>
+        <v/>
+      </c>
+      <c r="O27">
+        <f t="shared" si="12"/>
+        <v>20025</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="13"/>
+        <v>10025</v>
+      </c>
+      <c r="R27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U27" s="12">
+        <v>2</v>
+      </c>
+      <c r="V27" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W27" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28">
+        <f>A26+1</f>
+        <v>24</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f>IF(C26=C28,"",_xlfn.CONCAT("create transient schema if not exists ",B28," data_retention_time_in_days=0;  create or replace table ",B28,".",C28," as select"))</f>
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="5"/>
+        <v>column113</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="6"/>
+        <v>null::integer as column113</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="8"/>
+        <v>10000</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="9"/>
+        <v>integer</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="O28">
+        <f t="shared" si="12"/>
+        <v>20026</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="13"/>
+        <v>10026</v>
+      </c>
+      <c r="R28" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="U28" s="12">
+        <v>0</v>
+      </c>
+      <c r="V28" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4163,13 +4403,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD38527B-8DA9-F048-9888-D8112A4B2F49}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G26"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4353,11 +4593,12 @@
 IF(AND(L3="bigint",H3=K3),"seq8()",
 IF(AND(L3="char",H3=K3),_xlfn.CONCAT("rpad(seq8()::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H3," , random(",P3,")),current_date)"),
+IF(L3="boolean",_xlfn.CONCAT("(uniform(1,",H3,",random(",P3,"))-1)"),
 IF(OR(OR(OR(OR(L3="bigint",L3="double"),L3="integer"),L3="number"),L3="float"),_xlfn.CONCAT("uniform(1,",H3," , random(",P3,"))"),
 IF(L3="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H3,", random(",P3,"))))"),
 IF(L3="char",_xlfn.CONCAT("rpad(uniform(1,",H3," , random(",P3,"))::varchar,",M3,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L3="varchar",_xlfn.CONCAT("randstr(uniform(1,",M3,", random(",P3,")),uniform(1,",H3,",random(",P3,")))"),
-"")))))))))),"::",L3,
+""))))))))))),"::",L3,
 IF(OR(L3="varchar",L3="char"),_xlfn.CONCAT("(",M3,")"),
 IF(L3="number",_xlfn.CONCAT("(",M3,",",N3,")"),"")),
 " as ",F3)</f>
@@ -4436,11 +4677,11 @@
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B26" si="1">R4</f>
+        <f t="shared" ref="B4:B28" si="1">R4</f>
         <v>schema1</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C26" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
+        <f t="shared" ref="C4:C28" si="2">_xlfn.CONCAT($C$2,S4,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D4" s="4" t="str">
@@ -4448,68 +4689,69 @@
         <v/>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E26" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
+        <f t="shared" ref="E4:E28" si="4">IF(C4=C5,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K4,"))"))</f>
         <v/>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F26" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
+        <f t="shared" ref="F4:F28" si="5">_xlfn.CONCAT($F$2,T4,$F$2)</f>
         <v>column2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G26" si="6">_xlfn.CONCAT(
+        <f t="shared" ref="G4:G28" si="6">_xlfn.CONCAT(
 IF(H4=0,"null",
 IF(AND(L4="bigint",Q4=1),_xlfn.CONCAT("abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))"),
 IF(AND(L4="char",Q4=1),_xlfn.CONCAT("rpad(abs(trunc((5+normal(0,1,random(",P4,")))*(",H4,"/20)))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(AND(L4="bigint",H4=K4),"seq8()",
 IF(AND(L4="char",H4=K4),_xlfn.CONCAT("rpad(seq8()::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="date",_xlfn.CONCAT("dateadd(day,uniform(1,",H4," , random(",P4,")),current_date)"),
+IF(L4="boolean",_xlfn.CONCAT("(uniform(1,",H4,",random(",P4,"))-1)"),
 IF(OR(OR(OR(OR(L4="bigint",L4="double"),L4="integer"),L4="number"),L4="float"),_xlfn.CONCAT("uniform(1,",H4," , random(",P4,"))"),
 IF(L4="timestamp",_xlfn.CONCAT("(date_part(epoch_second, current_date)+(uniform(1,",H4,", random(",P4,"))))"),
 IF(L4="char",_xlfn.CONCAT("rpad(uniform(1,",H4," , random(",P4,"))::varchar,",M4,",'abcdefghifklmnopqrstuvwxyz')"),
 IF(L4="varchar",_xlfn.CONCAT("randstr(uniform(1,",M4,", random(",P4,")),uniform(1,",H4,",random(",P4,")))"),
-"")))))))))),"::",L4,
+""))))))))))),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10002))))::timestamp as column2</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H26" si="7">U4</f>
+        <f t="shared" ref="H4:H28" si="7">U4</f>
         <v>1234</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I26" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
+        <f t="shared" ref="I4:I28" si="8">_xlfn.CONCAT(IF(J4=0,F4,_xlfn.CONCAT("(case when uniform(1,1000,random(",O4,")) &gt; ",J4," then ",F4," else null end)")),"::",L4,
 IF(OR(L4="varchar",L4="char"),_xlfn.CONCAT("(",M4,")"),
 IF(L4="number",_xlfn.CONCAT("(",M4,",",N4,")"),"")),
 " as ",F4)</f>
         <v>column2::timestamp as column2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J26" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
+        <f t="shared" ref="J4:J28" si="9">IF(ISBLANK(Z4),0,IF(TRIM(Z4)="",0,INT((Z4/V4)*1000)))</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K26" si="10">V4</f>
+        <f t="shared" ref="K4:K28" si="10">V4</f>
         <v>10000</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L26" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
+        <f t="shared" ref="L4:L28" si="11">IF(OR(OR(W4="timestamp(3)",W4="timestamp(6)"),W4="timestamp(9)"),"TIMESTAMP",W4)</f>
         <v>timestamp</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M26" si="12">IF(ISBLANK(X4),"",X4)</f>
+        <f t="shared" ref="M4:M28" si="12">IF(ISBLANK(X4),"",X4)</f>
         <v/>
       </c>
       <c r="N4" t="str">
-        <f t="shared" ref="N4:N26" si="13">IF(ISBLANK(Y4),"",Y4)</f>
+        <f t="shared" ref="N4:N28" si="13">IF(ISBLANK(Y4),"",Y4)</f>
         <v/>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O26" si="14">O3+1</f>
+        <f t="shared" ref="O4:O28" si="14">O3+1</f>
         <v>20002</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P26" si="15">P3+1</f>
+        <f t="shared" ref="P4:P28" si="15">P3+1</f>
         <v>10002</v>
       </c>
       <c r="R4" s="12" t="s">
@@ -5385,19 +5627,19 @@
     </row>
     <row r="14" spans="1:30">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>A12+1</f>
+        <v>11</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B14" si="16">R14</f>
         <v>schema1</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C14" si="17">_xlfn.CONCAT($C$2,S14,$C$2)</f>
         <v>table1</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C12=C14,"",_xlfn.CONCAT("create transient schema if not exists ",B14," data_retention_time_in_days=0;  create or replace table ",B14,".",C14," as select"))</f>
         <v/>
       </c>
       <c r="E14" t="str">
@@ -5405,39 +5647,42 @@
         <v/>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F14" si="18">_xlfn.CONCAT($F$2,T14,$F$2)</f>
         <v>column12</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column12</v>
+        <v>(uniform(1,2,random(10012))-1)::boolean as column12</v>
       </c>
       <c r="H14">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="H14" si="19">U14</f>
+        <v>2</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ref="I14" si="20">_xlfn.CONCAT(IF(J14=0,F14,_xlfn.CONCAT("(case when uniform(1,1000,random(",O14,")) &gt; ",J14," then ",F14," else null end)")),"::",L14,
+IF(OR(L14="varchar",L14="char"),_xlfn.CONCAT("(",M14,")"),
+IF(L14="number",_xlfn.CONCAT("(",M14,",",N14,")"),"")),
+" as ",F14)</f>
+        <v>column12::boolean as column12</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14" si="21">IF(ISBLANK(Z14),0,IF(TRIM(Z14)="",0,INT((Z14/V14)*1000)))</f>
         <v>0</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="8"/>
-        <v>column12::integer as column12</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
       <c r="K14">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K14" si="22">V14</f>
         <v>10000</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="11"/>
-        <v>integer</v>
+        <f t="shared" ref="L14" si="23">IF(OR(OR(W14="timestamp(3)",W14="timestamp(6)"),W14="timestamp(9)"),"TIMESTAMP",W14)</f>
+        <v>boolean</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="M14" si="24">IF(ISBLANK(X14),"",X14)</f>
         <v/>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="N14" si="25">IF(ISBLANK(Y14),"",Y14)</f>
         <v/>
       </c>
       <c r="O14">
@@ -5458,13 +5703,13 @@
         <v>81</v>
       </c>
       <c r="U14" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="12">
         <v>10000</v>
       </c>
       <c r="W14" s="12" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
@@ -5478,8 +5723,8 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>A13+1</f>
+        <v>12</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="1"/>
@@ -5490,7 +5735,7 @@
         <v>table1</v>
       </c>
       <c r="D15" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(C13=C15,"",_xlfn.CONCAT("create transient schema if not exists ",B15," data_retention_time_in_days=0;  create or replace table ",B15,".",C15," as select"))</f>
         <v/>
       </c>
       <c r="E15" t="str">
@@ -5499,23 +5744,23 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="5"/>
-        <v>column101</v>
+        <v>column13</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="6"/>
-        <v>dateadd(day,uniform(1,1234 , random(10013)),current_date)::date as column101</v>
+        <v>null::integer as column13</v>
       </c>
       <c r="H15">
         <f t="shared" si="7"/>
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20013)) &gt; 300 then column101 else null end)::date as column101</v>
+        <v>column13::integer as column13</v>
       </c>
       <c r="J15">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="10"/>
@@ -5523,7 +5768,7 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="11"/>
-        <v>date</v>
+        <v>integer</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="12"/>
@@ -5548,21 +5793,21 @@
         <v>48</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="U15" s="12">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="V15" s="12">
         <v>10000</v>
       </c>
       <c r="W15" s="12" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
-      <c r="Z15" s="12">
-        <v>3000</v>
+      <c r="Z15" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
@@ -5572,7 +5817,7 @@
     <row r="16" spans="1:30">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="1"/>
@@ -5592,11 +5837,11 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="5"/>
-        <v>column102</v>
+        <v>column101</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="6"/>
-        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10014))))::timestamp as column102</v>
+        <v>dateadd(day,uniform(1,1234 , random(10014)),current_date)::date as column101</v>
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
@@ -5604,7 +5849,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20014)) &gt; 300 then column102 else null end)::timestamp as column102</v>
+        <v>(case when uniform(1,1000,random(20014)) &gt; 300 then column101 else null end)::date as column101</v>
       </c>
       <c r="J16">
         <f t="shared" si="9"/>
@@ -5616,7 +5861,7 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="11"/>
-        <v>timestamp</v>
+        <v>date</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="12"/>
@@ -5641,7 +5886,7 @@
         <v>48</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="U16" s="12">
         <v>1234</v>
@@ -5650,7 +5895,7 @@
         <v>10000</v>
       </c>
       <c r="W16" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -5665,7 +5910,7 @@
     <row r="17" spans="1:30">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="1"/>
@@ -5685,11 +5930,11 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="5"/>
-        <v>column103</v>
+        <v>column102</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="6"/>
-        <v>randstr(uniform(1,10, random(10015)),uniform(1,1234,random(10015)))::varchar(10) as column103</v>
+        <v>(date_part(epoch_second, current_date)+(uniform(1,1234, random(10015))))::timestamp as column102</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
@@ -5697,7 +5942,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20015)) &gt; 300 then column103 else null end)::varchar(10) as column103</v>
+        <v>(case when uniform(1,1000,random(20015)) &gt; 300 then column102 else null end)::timestamp as column102</v>
       </c>
       <c r="J17">
         <f t="shared" si="9"/>
@@ -5709,11 +5954,11 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="11"/>
-        <v>varchar</v>
-      </c>
-      <c r="M17">
+        <v>timestamp</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v/>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="13"/>
@@ -5734,7 +5979,7 @@
         <v>48</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U17" s="12">
         <v>1234</v>
@@ -5743,11 +5988,9 @@
         <v>10000</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="X17" s="12">
-        <v>10</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12">
         <v>3000</v>
@@ -5760,7 +6003,7 @@
     <row r="18" spans="1:30">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="1"/>
@@ -5780,11 +6023,11 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="5"/>
-        <v>column104</v>
+        <v>column103</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(uniform(1,1234 , random(10016))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
+        <v>randstr(uniform(1,10, random(10016)),uniform(1,1234,random(10016)))::varchar(10) as column103</v>
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
@@ -5792,7 +6035,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20016)) &gt; 300 then column104 else null end)::char(10) as column104</v>
+        <v>(case when uniform(1,1000,random(20016)) &gt; 300 then column103 else null end)::varchar(10) as column103</v>
       </c>
       <c r="J18">
         <f t="shared" si="9"/>
@@ -5804,7 +6047,7 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="11"/>
-        <v>char</v>
+        <v>varchar</v>
       </c>
       <c r="M18">
         <f t="shared" si="12"/>
@@ -5829,7 +6072,7 @@
         <v>48</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U18" s="12">
         <v>1234</v>
@@ -5838,7 +6081,7 @@
         <v>10000</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X18" s="12">
         <v>10</v>
@@ -5855,7 +6098,7 @@
     <row r="19" spans="1:30">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="1"/>
@@ -5875,11 +6118,11 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="5"/>
-        <v>column105</v>
+        <v>column104</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10017))::bigint as column105</v>
+        <v>rpad(uniform(1,1234 , random(10017))::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column104</v>
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
@@ -5887,7 +6130,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20017)) &gt; 300 then column105 else null end)::bigint as column105</v>
+        <v>(case when uniform(1,1000,random(20017)) &gt; 300 then column104 else null end)::char(10) as column104</v>
       </c>
       <c r="J19">
         <f t="shared" si="9"/>
@@ -5899,11 +6142,11 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M19" t="str">
+        <v>char</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="13"/>
@@ -5924,7 +6167,7 @@
         <v>48</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U19" s="12">
         <v>1234</v>
@@ -5933,9 +6176,11 @@
         <v>10000</v>
       </c>
       <c r="W19" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="X19" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="X19" s="12">
+        <v>10</v>
+      </c>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12">
         <v>3000</v>
@@ -5948,7 +6193,7 @@
     <row r="20" spans="1:30">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="1"/>
@@ -5968,11 +6213,11 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="5"/>
-        <v>column106</v>
+        <v>column105</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10018))::integer as column106</v>
+        <v>uniform(1,1234 , random(10018))::bigint as column105</v>
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
@@ -5980,7 +6225,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20018)) &gt; 300 then column106 else null end)::integer as column106</v>
+        <v>(case when uniform(1,1000,random(20018)) &gt; 300 then column105 else null end)::bigint as column105</v>
       </c>
       <c r="J20">
         <f t="shared" si="9"/>
@@ -5992,7 +6237,7 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="11"/>
-        <v>integer</v>
+        <v>bigint</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="12"/>
@@ -6017,7 +6262,7 @@
         <v>48</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="U20" s="12">
         <v>1234</v>
@@ -6026,7 +6271,7 @@
         <v>10000</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
@@ -6041,7 +6286,7 @@
     <row r="21" spans="1:30">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="1"/>
@@ -6061,11 +6306,11 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="5"/>
-        <v>column107</v>
+        <v>column106</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10019))::double as column107</v>
+        <v>uniform(1,1234 , random(10019))::integer as column106</v>
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
@@ -6073,7 +6318,7 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20019)) &gt; 300 then column107 else null end)::double as column107</v>
+        <v>(case when uniform(1,1000,random(20019)) &gt; 300 then column106 else null end)::integer as column106</v>
       </c>
       <c r="J21">
         <f t="shared" si="9"/>
@@ -6085,7 +6330,7 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="11"/>
-        <v>double</v>
+        <v>integer</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="12"/>
@@ -6110,7 +6355,7 @@
         <v>48</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U21" s="12">
         <v>1234</v>
@@ -6119,7 +6364,7 @@
         <v>10000</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
@@ -6134,7 +6379,7 @@
     <row r="22" spans="1:30">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="1"/>
@@ -6154,11 +6399,11 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="5"/>
-        <v>column108</v>
+        <v>column107</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10020))::float as column108</v>
+        <v>uniform(1,1234 , random(10020))::double as column107</v>
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
@@ -6166,7 +6411,7 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20020)) &gt; 300 then column108 else null end)::float as column108</v>
+        <v>(case when uniform(1,1000,random(20020)) &gt; 300 then column107 else null end)::double as column107</v>
       </c>
       <c r="J22">
         <f t="shared" si="9"/>
@@ -6178,7 +6423,7 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="11"/>
-        <v>float</v>
+        <v>double</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="12"/>
@@ -6203,7 +6448,7 @@
         <v>48</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U22" s="12">
         <v>1234</v>
@@ -6212,7 +6457,7 @@
         <v>10000</v>
       </c>
       <c r="W22" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
@@ -6227,7 +6472,7 @@
     <row r="23" spans="1:30">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="1"/>
@@ -6247,11 +6492,11 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="5"/>
-        <v>column109</v>
+        <v>column108</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="6"/>
-        <v>uniform(1,1234 , random(10021))::number(10,2) as column109</v>
+        <v>uniform(1,1234 , random(10021))::float as column108</v>
       </c>
       <c r="H23">
         <f t="shared" si="7"/>
@@ -6259,7 +6504,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20021)) &gt; 300 then column109 else null end)::number(10,2) as column109</v>
+        <v>(case when uniform(1,1000,random(20021)) &gt; 300 then column108 else null end)::float as column108</v>
       </c>
       <c r="J23">
         <f t="shared" si="9"/>
@@ -6271,15 +6516,15 @@
       </c>
       <c r="L23" t="str">
         <f t="shared" si="11"/>
-        <v>number</v>
-      </c>
-      <c r="M23">
+        <v>float</v>
+      </c>
+      <c r="M23" t="str">
         <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="N23">
+        <v/>
+      </c>
+      <c r="N23" t="str">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="O23">
         <f t="shared" si="14"/>
@@ -6296,7 +6541,7 @@
         <v>48</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U23" s="12">
         <v>1234</v>
@@ -6305,14 +6550,10 @@
         <v>10000</v>
       </c>
       <c r="W23" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="X23" s="12">
-        <v>10</v>
-      </c>
-      <c r="Y23" s="12">
-        <v>2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
       <c r="Z23" s="12">
         <v>3000</v>
       </c>
@@ -6324,7 +6565,7 @@
     <row r="24" spans="1:30">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="1"/>
@@ -6344,19 +6585,19 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="5"/>
-        <v>column110</v>
+        <v>column109</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="6"/>
-        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
+        <v>uniform(1,1234 , random(10022))::number(10,2) as column109</v>
       </c>
       <c r="H24">
         <f t="shared" si="7"/>
-        <v>10000</v>
+        <v>1234</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20022)) &gt; 300 then column110 else null end)::char(10) as column110</v>
+        <v>(case when uniform(1,1000,random(20022)) &gt; 300 then column109 else null end)::number(10,2) as column109</v>
       </c>
       <c r="J24">
         <f t="shared" si="9"/>
@@ -6368,15 +6609,15 @@
       </c>
       <c r="L24" t="str">
         <f t="shared" si="11"/>
-        <v>char</v>
+        <v>number</v>
       </c>
       <c r="M24">
         <f t="shared" si="12"/>
         <v>10</v>
       </c>
-      <c r="N24" t="str">
+      <c r="N24">
         <f t="shared" si="13"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="O24">
         <f t="shared" si="14"/>
@@ -6386,28 +6627,30 @@
         <f t="shared" si="15"/>
         <v>10022</v>
       </c>
-      <c r="R24" s="13" t="s">
+      <c r="R24" s="12" t="s">
         <v>47</v>
       </c>
       <c r="S24" s="12" t="s">
         <v>48</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U24" s="12">
-        <v>10000</v>
+        <v>1234</v>
       </c>
       <c r="V24" s="12">
         <v>10000</v>
       </c>
       <c r="W24" s="12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="X24" s="12">
         <v>10</v>
       </c>
-      <c r="Y24" s="12"/>
+      <c r="Y24" s="12">
+        <v>2</v>
+      </c>
       <c r="Z24" s="12">
         <v>3000</v>
       </c>
@@ -6419,7 +6662,7 @@
     <row r="25" spans="1:30">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="1"/>
@@ -6439,11 +6682,11 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="5"/>
-        <v>column111</v>
+        <v>column110</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="6"/>
-        <v>seq8()::bigint as column111</v>
+        <v>rpad(seq8()::varchar,10,'abcdefghifklmnopqrstuvwxyz')::char(10) as column110</v>
       </c>
       <c r="H25">
         <f t="shared" si="7"/>
@@ -6451,7 +6694,7 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20023)) &gt; 300 then column111 else null end)::bigint as column111</v>
+        <v>(case when uniform(1,1000,random(20023)) &gt; 300 then column110 else null end)::char(10) as column110</v>
       </c>
       <c r="J25">
         <f t="shared" si="9"/>
@@ -6463,11 +6706,11 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="11"/>
-        <v>bigint</v>
-      </c>
-      <c r="M25" t="str">
+        <v>char</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="12"/>
-        <v/>
+        <v>10</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="13"/>
@@ -6481,14 +6724,14 @@
         <f t="shared" si="15"/>
         <v>10023</v>
       </c>
-      <c r="R25" s="12" t="s">
+      <c r="R25" s="13" t="s">
         <v>47</v>
       </c>
       <c r="S25" s="12" t="s">
         <v>48</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="U25" s="12">
         <v>10000</v>
@@ -6496,10 +6739,12 @@
       <c r="V25" s="12">
         <v>10000</v>
       </c>
-      <c r="W25" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="X25" s="12"/>
+      <c r="W25" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="X25" s="12">
+        <v>10</v>
+      </c>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12">
         <v>3000</v>
@@ -6512,7 +6757,7 @@
     <row r="26" spans="1:30">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="1"/>
@@ -6528,23 +6773,23 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="4"/>
-        <v>from table(generator(rowcount =&gt; 10000))</v>
+        <v/>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="5"/>
-        <v>column112</v>
+        <v>column111</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="6"/>
-        <v>null::integer as column112</v>
+        <v>seq8()::bigint as column111</v>
       </c>
       <c r="H26">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="8"/>
-        <v>(case when uniform(1,1000,random(20024)) &gt; 300 then column112 else null end)::integer as column112</v>
+        <v>(case when uniform(1,1000,random(20024)) &gt; 300 then column111 else null end)::bigint as column111</v>
       </c>
       <c r="J26">
         <f t="shared" si="9"/>
@@ -6556,7 +6801,7 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="11"/>
-        <v>integer</v>
+        <v>bigint</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="12"/>
@@ -6581,16 +6826,16 @@
         <v>48</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U26" s="12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V26" s="12">
         <v>10000</v>
       </c>
-      <c r="W26" s="12" t="s">
-        <v>59</v>
+      <c r="W26" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
@@ -6602,8 +6847,197 @@
       <c r="AC26" s="12"/>
       <c r="AD26" s="12"/>
     </row>
+    <row r="27" spans="1:30">
+      <c r="A27">
+        <f>A25+1</f>
+        <v>23</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ref="B27" si="26">R27</f>
+        <v>schema1</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ref="C27" si="27">_xlfn.CONCAT($C$2,S27,$C$2)</f>
+        <v>table1</v>
+      </c>
+      <c r="D27" s="4" t="str">
+        <f>IF(C25=C27,"",_xlfn.CONCAT("create transient schema if not exists ",B27," data_retention_time_in_days=0;  create or replace table ",B27,".",C27," as select"))</f>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" ref="E27" si="28">IF(C27=C28,"",_xlfn.CONCAT("from table(generator(rowcount =&gt; ",K27,"))"))</f>
+        <v/>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" ref="F27" si="29">_xlfn.CONCAT($F$2,T27,$F$2)</f>
+        <v>column112</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="6"/>
+        <v>(uniform(1,2,random(10025))-1)::boolean as column112</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27" si="30">U27</f>
+        <v>2</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" ref="I27" si="31">_xlfn.CONCAT(IF(J27=0,F27,_xlfn.CONCAT("(case when uniform(1,1000,random(",O27,")) &gt; ",J27," then ",F27," else null end)")),"::",L27,
+IF(OR(L27="varchar",L27="char"),_xlfn.CONCAT("(",M27,")"),
+IF(L27="number",_xlfn.CONCAT("(",M27,",",N27,")"),"")),
+" as ",F27)</f>
+        <v>(case when uniform(1,1000,random(20025)) &gt; 300 then column112 else null end)::boolean as column112</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27" si="32">IF(ISBLANK(Z27),0,IF(TRIM(Z27)="",0,INT((Z27/V27)*1000)))</f>
+        <v>300</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27" si="33">V27</f>
+        <v>10000</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" ref="L27" si="34">IF(OR(OR(W27="timestamp(3)",W27="timestamp(6)"),W27="timestamp(9)"),"TIMESTAMP",W27)</f>
+        <v>boolean</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" ref="M27" si="35">IF(ISBLANK(X27),"",X27)</f>
+        <v/>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" ref="N27" si="36">IF(ISBLANK(Y27),"",Y27)</f>
+        <v/>
+      </c>
+      <c r="O27">
+        <f t="shared" si="14"/>
+        <v>20025</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="15"/>
+        <v>10025</v>
+      </c>
+      <c r="R27" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U27" s="12">
+        <v>2</v>
+      </c>
+      <c r="V27" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W27" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28">
+        <f>A26+1</f>
+        <v>24</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>schema1</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="2"/>
+        <v>table1</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f>IF(C26=C28,"",_xlfn.CONCAT("create transient schema if not exists ",B28," data_retention_time_in_days=0;  create or replace table ",B28,".",C28," as select"))</f>
+        <v/>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="4"/>
+        <v>from table(generator(rowcount =&gt; 10000))</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="5"/>
+        <v>column113</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="6"/>
+        <v>null::integer as column113</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="8"/>
+        <v>(case when uniform(1,1000,random(20026)) &gt; 300 then column113 else null end)::integer as column113</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="10"/>
+        <v>10000</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="11"/>
+        <v>integer</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="O28">
+        <f t="shared" si="14"/>
+        <v>20026</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="15"/>
+        <v>10026</v>
+      </c>
+      <c r="R28" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="T28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="U28" s="12">
+        <v>0</v>
+      </c>
+      <c r="V28" s="12">
+        <v>10000</v>
+      </c>
+      <c r="W28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12">
+        <v>3000</v>
+      </c>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AD28" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AD177" xr:uid="{1DEE4BB0-2492-0346-9743-0CF6D1D58AA5}"/>
+  <autoFilter ref="A1:AD179" xr:uid="{1DEE4BB0-2492-0346-9743-0CF6D1D58AA5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7212,294 +7646,294 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>